<commit_message>
Fix tolls file for USE=1
And USE=4 for express lanes
</commit_message>
<xml_diff>
--- a/hwy/Tolls_TM1.5.xlsx
+++ b/hwy/Tolls_TM1.5.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftsang\Box\Modeling and Surveys\Development\Travel Model 1.5\Model_inputs\2015\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\hwy\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ACA069-AC6A-4E12-9241-4D45615DFCEA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11625" tabRatio="858" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11625" tabRatio="858" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" tolls 2010 NOT USED" sheetId="1" r:id="rId1"/>
@@ -29,22 +30,28 @@
     <definedName name="CPI_2015_to_2010" localSheetId="2">'tolls 2015 (wsp) NOT USED'!$C$47</definedName>
     <definedName name="CPI_2015_to_2010">'tolls 2015'!$B$27</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Flavia Tsang</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -920,7 +927,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -1568,7 +1575,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1628,7 +1641,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1680,7 +1699,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EC9DBF03-1652-45AC-BAE5-60A830A343AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC9DBF03-1652-45AC-BAE5-60A830A343AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1728,7 +1747,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8543A9F4-5207-4914-A667-5ACB39771DFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8543A9F4-5207-4914-A667-5ACB39771DFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1776,7 +1795,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3FB7EF22-B7FB-42C2-B140-4D5A64BAB2EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB7EF22-B7FB-42C2-B140-4D5A64BAB2EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2100,7 +2119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3687,7 +3706,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B43:K45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3726,7 +3745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B42"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -3747,7 +3766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -4316,7 +4335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
@@ -7601,7 +7620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10282,14 +10301,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:Z41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10424,7 +10443,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5">
         <v>5</v>
@@ -10568,7 +10587,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5">
         <v>5</v>
@@ -10707,7 +10726,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="5">
         <v>5</v>
@@ -10851,7 +10870,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="5">
         <v>5</v>
@@ -10995,7 +11014,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="5">
         <v>4</v>
@@ -11134,7 +11153,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="5">
         <v>6.75</v>
@@ -11278,7 +11297,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="5">
         <v>5</v>
@@ -11422,7 +11441,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="5">
         <v>5</v>
@@ -11947,15 +11966,15 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:AO20"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12127,7 +12146,7 @@
       </c>
       <c r="B2" s="1">
         <f>C2*1000+D2*10+F2</f>
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="C2" s="1">
         <f>'tolls 2015'!C4</f>
@@ -12142,7 +12161,7 @@
       </c>
       <c r="F2" s="1">
         <f>'tolls 2015'!F4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="5">
         <f>IF('tolls 2015'!G4="n/a",0,'tolls 2015'!G4)*CPI_2015_to_2010</f>
@@ -12457,7 +12476,7 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C4" s="1">
         <f>'tolls 2015'!C6</f>
@@ -12472,7 +12491,7 @@
       </c>
       <c r="F4" s="1">
         <f>'tolls 2015'!F6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5">
         <f>IF('tolls 2015'!G6="n/a",0,'tolls 2015'!G6)*CPI_2015_to_2010</f>
@@ -12787,7 +12806,7 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>8001</v>
       </c>
       <c r="C6" s="1">
         <f>'tolls 2015'!C8</f>
@@ -12802,7 +12821,7 @@
       </c>
       <c r="F6" s="1">
         <f>'tolls 2015'!F8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5">
         <f>IF('tolls 2015'!G8="n/a",0,'tolls 2015'!G8)*CPI_2015_to_2010</f>
@@ -13117,7 +13136,7 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>3001</v>
       </c>
       <c r="C8" s="1">
         <f>'tolls 2015'!C10</f>
@@ -13132,7 +13151,7 @@
       </c>
       <c r="F8" s="1">
         <f>'tolls 2015'!F10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="5">
         <f>IF('tolls 2015'!G10="n/a",0,'tolls 2015'!G10)*CPI_2015_to_2010</f>
@@ -13447,7 +13466,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>5001</v>
       </c>
       <c r="C10" s="1">
         <f>'tolls 2015'!C12</f>
@@ -13462,7 +13481,7 @@
       </c>
       <c r="F10" s="1">
         <f>'tolls 2015'!F12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="5">
         <f>IF('tolls 2015'!G12="n/a",0,'tolls 2015'!G12)*CPI_2015_to_2010</f>
@@ -13777,7 +13796,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>4001</v>
       </c>
       <c r="C12" s="1">
         <f>'tolls 2015'!C14</f>
@@ -13792,7 +13811,7 @@
       </c>
       <c r="F12" s="1">
         <f>'tolls 2015'!F14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="5">
         <f>IF('tolls 2015'!G14="n/a",0,'tolls 2015'!G14)*CPI_2015_to_2010</f>
@@ -14107,7 +14126,7 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>6001</v>
       </c>
       <c r="C14" s="1">
         <f>'tolls 2015'!C16</f>
@@ -14122,7 +14141,7 @@
       </c>
       <c r="F14" s="1">
         <f>'tolls 2015'!F16</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="5">
         <f>IF('tolls 2015'!G16="n/a",0,'tolls 2015'!G16)*CPI_2015_to_2010</f>
@@ -14437,7 +14456,7 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>7000</v>
+        <v>7001</v>
       </c>
       <c r="C16" s="1">
         <f>'tolls 2015'!C18</f>
@@ -14452,7 +14471,7 @@
       </c>
       <c r="F16" s="1">
         <f>'tolls 2015'!F18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="5">
         <f>IF('tolls 2015'!G18="n/a",0,'tolls 2015'!G18)*CPI_2015_to_2010</f>
@@ -15256,7 +15275,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
@@ -15436,7 +15455,7 @@
       </c>
       <c r="B2" s="1">
         <f>C2*1000+D2*10+F2</f>
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="C2" s="1">
         <f>'tolls 2015'!C4</f>
@@ -15451,7 +15470,7 @@
       </c>
       <c r="F2" s="1">
         <f>'tolls 2015'!F4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="5">
         <f>IF('tolls 2015'!G4="n/a",0,'tolls 2015'!G4)*CPI_2015_to_2010</f>
@@ -15766,7 +15785,7 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="C4" s="1">
         <f>'tolls 2015'!C6</f>
@@ -15781,7 +15800,7 @@
       </c>
       <c r="F4" s="1">
         <f>'tolls 2015'!F6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5">
         <f>IF('tolls 2015'!G6="n/a",0,'tolls 2015'!G6)*CPI_2015_to_2010</f>
@@ -16096,7 +16115,7 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>8001</v>
       </c>
       <c r="C6" s="1">
         <f>'tolls 2015'!C8</f>
@@ -16111,7 +16130,7 @@
       </c>
       <c r="F6" s="1">
         <f>'tolls 2015'!F8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="5">
         <f>IF('tolls 2015'!G8="n/a",0,'tolls 2015'!G8)*CPI_2015_to_2010</f>
@@ -16426,7 +16445,7 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>3001</v>
       </c>
       <c r="C8" s="1">
         <f>'tolls 2015'!C10</f>
@@ -16441,7 +16460,7 @@
       </c>
       <c r="F8" s="1">
         <f>'tolls 2015'!F10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="5">
         <f>IF('tolls 2015'!G10="n/a",0,'tolls 2015'!G10)*CPI_2015_to_2010</f>
@@ -16756,7 +16775,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>5001</v>
       </c>
       <c r="C10" s="1">
         <f>'tolls 2015'!C12</f>
@@ -16771,7 +16790,7 @@
       </c>
       <c r="F10" s="1">
         <f>'tolls 2015'!F12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="5">
         <f>IF('tolls 2015'!G12="n/a",0,'tolls 2015'!G12)*CPI_2015_to_2010</f>
@@ -17086,7 +17105,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>4001</v>
       </c>
       <c r="C12" s="1">
         <f>'tolls 2015'!C14</f>
@@ -17101,7 +17120,7 @@
       </c>
       <c r="F12" s="1">
         <f>'tolls 2015'!F14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="5">
         <f>IF('tolls 2015'!G14="n/a",0,'tolls 2015'!G14)*CPI_2015_to_2010</f>
@@ -17416,7 +17435,7 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>6001</v>
       </c>
       <c r="C14" s="1">
         <f>'tolls 2015'!C16</f>
@@ -17431,7 +17450,7 @@
       </c>
       <c r="F14" s="1">
         <f>'tolls 2015'!F16</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="5">
         <f>IF('tolls 2015'!G16="n/a",0,'tolls 2015'!G16)*CPI_2015_to_2010</f>
@@ -17746,7 +17765,7 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>7000</v>
+        <v>7001</v>
       </c>
       <c r="C16" s="1">
         <f>'tolls 2015'!C18</f>
@@ -17761,7 +17780,7 @@
       </c>
       <c r="F16" s="1">
         <f>'tolls 2015'!F18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="5">
         <f>IF('tolls 2015'!G18="n/a",0,'tolls 2015'!G18)*CPI_2015_to_2010</f>
@@ -20965,7 +20984,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20991,7 +21010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21028,7 +21047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Add column, toll_flat to distinguish between distance-based and flat tolls
</commit_message>
<xml_diff>
--- a/hwy/Tolls_TM1.5.xlsx
+++ b/hwy/Tolls_TM1.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\hwy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1739F4-5ECE-4C79-8A7B-6985C16EA9D3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FC4A3F-1B7E-4122-91A3-AE42A9E62AF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="11625" tabRatio="858" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="2040" windowWidth="26205" windowHeight="11565" tabRatio="858" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" tolls 2010 NOT USED" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="201">
   <si>
     <t>TollBooth</t>
   </si>
@@ -923,6 +923,9 @@
   <si>
     <t>Tolls expressed in 2015$ on this page. Prices in TM1.5 are in 2000$. Inflation factors are applied on the next page.</t>
   </si>
+  <si>
+    <t>toll_flat</t>
+  </si>
 </sst>
 </file>
 
@@ -931,7 +934,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1112,8 +1115,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1195,6 +1206,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1301,7 +1318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1527,6 +1544,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11957,11 +11975,11 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:AO20"/>
+  <dimension ref="A1:AP20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomLeft" activeCell="AP5" sqref="AP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11998,10 +12016,11 @@
     <col min="38" max="38" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="39" max="40" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="1"/>
+    <col min="42" max="42" width="7.85546875" style="1" customWidth="1"/>
+    <col min="43" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>102</v>
       </c>
@@ -12125,8 +12144,11 @@
       <c r="AO1" s="36" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP1" s="101" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
         <f>'tolls 2015'!A4</f>
         <v>Carquinez Bridge GP</v>
@@ -12290,8 +12312,11 @@
         <f>AK2</f>
         <v>17.482517482517483</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
         <f>'tolls 2015'!A5</f>
         <v>Carquinez Bridge HOV</v>
@@ -12455,8 +12480,11 @@
         <f t="shared" ref="AO3:AO16" si="16">AK3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
         <f>'tolls 2015'!A6</f>
         <v>Benicia-Martinez Bridge GP</v>
@@ -12620,8 +12648,11 @@
         <f t="shared" si="16"/>
         <v>17.482517482517483</v>
       </c>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
         <f>'tolls 2015'!A7</f>
         <v>Benicia-Martinez Bridge HOV</v>
@@ -12785,8 +12816,11 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
         <f>'tolls 2015'!A8</f>
         <v>Antioch Bridge GP</v>
@@ -12950,8 +12984,11 @@
         <f t="shared" si="16"/>
         <v>7.8671328671328684</v>
       </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
         <f>'tolls 2015'!A9</f>
         <v>Antioch Bridge HOV</v>
@@ -13115,8 +13152,11 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
         <f>'tolls 2015'!A10</f>
         <v>Richmond-San Rafael Bridge GP</v>
@@ -13280,8 +13320,11 @@
         <f t="shared" si="16"/>
         <v>17.482517482517483</v>
       </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
         <f>'tolls 2015'!A11</f>
         <v>Richmond-San Rafael Bridge HOV</v>
@@ -13445,8 +13488,11 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="str">
         <f>'tolls 2015'!A12</f>
         <v>San Francisco Bay Bridge GP</v>
@@ -13610,8 +13656,11 @@
         <f t="shared" si="16"/>
         <v>7.8671328671328684</v>
       </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="str">
         <f>'tolls 2015'!A13</f>
         <v>San Francisco Bay Bridge HOV</v>
@@ -13775,8 +13824,11 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="str">
         <f>'tolls 2015'!A14</f>
         <v>Golden Gate Bridge GP</v>
@@ -13940,8 +13992,11 @@
         <f t="shared" si="16"/>
         <v>23.601398601398603</v>
       </c>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="str">
         <f>'tolls 2015'!A15</f>
         <v>Golden Gate Bridge HOV</v>
@@ -14105,8 +14160,11 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="str">
         <f>'tolls 2015'!A16</f>
         <v>San Mateo-Hayward Bridge GP</v>
@@ -14270,8 +14328,11 @@
         <f t="shared" si="16"/>
         <v>17.482517482517483</v>
       </c>
-    </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="str">
         <f>'tolls 2015'!A17</f>
         <v>San Mateo-Hayward Bridge HOV</v>
@@ -14435,8 +14496,11 @@
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="str">
         <f>'tolls 2015'!A18</f>
         <v>Dumbarton Bridge GP</v>
@@ -14600,8 +14664,11 @@
         <f t="shared" si="16"/>
         <v>17.482517482517483</v>
       </c>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="AP16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="str">
         <f>'tolls 2015'!A19</f>
         <v>Dumbarton Bridge HOV</v>
@@ -14765,8 +14832,11 @@
         <f t="shared" ref="AO17" si="28">AK17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:41" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AP17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="41" t="str">
         <f>"I-680 Sunol EL SB "&amp;'tolls 2015'!A21</f>
         <v>I-680 Sunol EL SB Entire length</v>
@@ -14929,8 +14999,11 @@
         <f>IF('tolls 2015'!K21="n/a",0,'tolls 2015'!K21)*CPI_2015_to_2000</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:41" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AP18" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="41" t="str">
         <f>"SR-237 EL SB "&amp;'tolls 2015'!A23</f>
         <v>SR-237 EL SB Entire length</v>
@@ -15092,8 +15165,11 @@
         <f>IF('tolls 2015'!K23="n/a",0,'tolls 2015'!K23)*CPI_2015_to_2000</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:41" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AP19" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="41" t="str">
         <f>"SR-237 EL NB "&amp;'tolls 2015'!A25</f>
         <v>SR-237 EL NB Entire length</v>
@@ -15255,9 +15331,13 @@
         <f>IF('tolls 2015'!K25="n/a",0,'tolls 2015'!K25)*CPI_2015_to_2000</f>
         <v>0</v>
       </c>
+      <c r="AP20" s="41">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added toll classes 887 and 888 (they're part of SR-237 Express Lanes)
</commit_message>
<xml_diff>
--- a/hwy/Tolls_TM1.5.xlsx
+++ b/hwy/Tolls_TM1.5.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\hwy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FC4A3F-1B7E-4122-91A3-AE42A9E62AF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="2040" windowWidth="26205" windowHeight="11565" tabRatio="858" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="2040" windowWidth="26205" windowHeight="11565" tabRatio="858" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name=" tolls 2010 NOT USED" sheetId="1" r:id="rId1"/>
@@ -27,10 +26,10 @@
     <sheet name="data from ACTC" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="CPI_2015_to_2000">'tolls 2015'!$B$27</definedName>
+    <definedName name="CPI_2015_to_2000">'tolls 2015'!$B$31</definedName>
     <definedName name="CPI_2015_to_2010" localSheetId="2">'tolls 2015 (wsp) NOT USED'!$C$47</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,12 +45,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Flavia Tsang</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="209">
   <si>
     <t>TollBooth</t>
   </si>
@@ -918,19 +917,43 @@
     <t>use</t>
   </si>
   <si>
-    <t>Entire length</t>
-  </si>
-  <si>
     <t>Tolls expressed in 2015$ on this page. Prices in TM1.5 are in 2000$. Inflation factors are applied on the next page.</t>
   </si>
   <si>
     <t>toll_flat</t>
   </si>
+  <si>
+    <t>US101 Interchange to I-880 Interchange</t>
+  </si>
+  <si>
+    <t>SCL County Line to SR84</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>SR-237 Express Lanes WB:</t>
+  </si>
+  <si>
+    <t>SR-237 Express Lanes EB:</t>
+  </si>
+  <si>
+    <t>SR-237 Express Lanes (last segment after TOLLCLASS 231):</t>
+  </si>
+  <si>
+    <t>SR-237 Express Lanes (first segment before TOLLCLASS 232):</t>
+  </si>
+  <si>
+    <t>I-880 SCL - SR237 to SR262 Mission Blvd - NB</t>
+  </si>
+  <si>
+    <t>I-880 SCL - SR237 to SR262 Mission Blvd - SB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -1318,7 +1341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1484,6 +1507,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1544,7 +1570,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1583,7 +1608,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1649,7 +1674,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1704,7 +1729,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC9DBF03-1652-45AC-BAE5-60A830A343AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EC9DBF03-1652-45AC-BAE5-60A830A343AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1752,7 +1777,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8543A9F4-5207-4914-A667-5ACB39771DFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8543A9F4-5207-4914-A667-5ACB39771DFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1800,7 +1825,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB7EF22-B7FB-42C2-B140-4D5A64BAB2EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3FB7EF22-B7FB-42C2-B140-4D5A64BAB2EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2124,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AA33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2148,34 +2173,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="86" t="s">
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="87" t="s">
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
-      <c r="V2" s="87"/>
-      <c r="W2" s="79" t="s">
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="79"/>
-      <c r="AA2" s="79"/>
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="82"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
@@ -3478,13 +3503,13 @@
       <c r="V21" s="17">
         <v>0</v>
       </c>
-      <c r="W21" s="80" t="s">
+      <c r="W21" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="X21" s="81"/>
-      <c r="Y21" s="81"/>
-      <c r="Z21" s="81"/>
-      <c r="AA21" s="81"/>
+      <c r="X21" s="84"/>
+      <c r="Y21" s="84"/>
+      <c r="Z21" s="84"/>
+      <c r="AA21" s="84"/>
     </row>
     <row r="22" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="16" t="s">
@@ -3548,11 +3573,11 @@
       <c r="V22" s="17">
         <v>0</v>
       </c>
-      <c r="W22" s="81"/>
-      <c r="X22" s="81"/>
-      <c r="Y22" s="81"/>
-      <c r="Z22" s="81"/>
-      <c r="AA22" s="81"/>
+      <c r="W22" s="84"/>
+      <c r="X22" s="84"/>
+      <c r="Y22" s="84"/>
+      <c r="Z22" s="84"/>
+      <c r="AA22" s="84"/>
     </row>
     <row r="23" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="16" t="s">
@@ -3616,11 +3641,11 @@
       <c r="V23" s="17">
         <v>0</v>
       </c>
-      <c r="W23" s="81"/>
-      <c r="X23" s="81"/>
-      <c r="Y23" s="81"/>
-      <c r="Z23" s="81"/>
-      <c r="AA23" s="81"/>
+      <c r="W23" s="84"/>
+      <c r="X23" s="84"/>
+      <c r="Y23" s="84"/>
+      <c r="Z23" s="84"/>
+      <c r="AA23" s="84"/>
     </row>
     <row r="24" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B24" s="11"/>
@@ -3639,49 +3664,49 @@
       </c>
     </row>
     <row r="28" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
-      <c r="K28" s="84"/>
-      <c r="L28" s="84"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="87"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
     </row>
     <row r="29" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="84" t="s">
+      <c r="B29" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="84"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="84"/>
-      <c r="J29" s="84"/>
-      <c r="K29" s="84"/>
-      <c r="L29" s="84"/>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
     </row>
     <row r="30" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B30" s="82" t="s">
+      <c r="B30" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="83"/>
-      <c r="J30" s="83"/>
-      <c r="K30" s="83"/>
-      <c r="L30" s="83"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="86"/>
+      <c r="I30" s="86"/>
+      <c r="J30" s="86"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="86"/>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B31" s="28" t="s">
@@ -3711,7 +3736,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B43:K45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3721,18 +3746,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="43" spans="2:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="92" t="s">
+      <c r="B43" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="93"/>
-      <c r="D43" s="93"/>
-      <c r="E43" s="93"/>
-      <c r="F43" s="93"/>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="93"/>
-      <c r="J43" s="93"/>
-      <c r="K43" s="93"/>
+      <c r="C43" s="96"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="96"/>
+      <c r="F43" s="96"/>
+      <c r="G43" s="96"/>
+      <c r="H43" s="96"/>
+      <c r="I43" s="96"/>
+      <c r="J43" s="96"/>
+      <c r="K43" s="96"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
@@ -3750,7 +3775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B42"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -3771,7 +3796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -3902,13 +3927,13 @@
     </row>
     <row r="14" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="54"/>
-      <c r="C14" s="94" t="s">
+      <c r="C14" s="97" t="s">
         <v>162</v>
       </c>
-      <c r="D14" s="95"/>
-      <c r="E14" s="95"/>
-      <c r="F14" s="95"/>
-      <c r="G14" s="96"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="99"/>
     </row>
     <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="55"/>
@@ -3919,10 +3944,10 @@
         <v>164</v>
       </c>
       <c r="E15" s="57"/>
-      <c r="F15" s="97" t="s">
+      <c r="F15" s="100" t="s">
         <v>165</v>
       </c>
-      <c r="G15" s="98"/>
+      <c r="G15" s="101"/>
     </row>
     <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="58" t="s">
@@ -4257,10 +4282,10 @@
         <v>10.18</v>
       </c>
       <c r="E35" s="66"/>
-      <c r="F35" s="99">
+      <c r="F35" s="102">
         <v>12.7</v>
       </c>
-      <c r="G35" s="100"/>
+      <c r="G35" s="103"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="53"/>
@@ -4340,7 +4365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
@@ -7126,7 +7151,7 @@
     <row r="18" spans="1:41" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="str">
         <f>"I-680 EL SB "&amp;'tolls 2015'!A21</f>
-        <v>I-680 EL SB Entire length</v>
+        <v>I-680 EL SB SCL County Line to SR84</v>
       </c>
       <c r="B18" s="29">
         <f>C18*1000+D18*10+F18</f>
@@ -7625,14 +7650,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7645,34 +7670,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="86" t="s">
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="87" t="s">
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
-      <c r="V2" s="87"/>
-      <c r="W2" s="79" t="s">
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="90"/>
+      <c r="W2" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="79"/>
-      <c r="AA2" s="79"/>
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="82"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
@@ -8969,13 +8994,13 @@
       <c r="V21" s="5">
         <v>0</v>
       </c>
-      <c r="W21" s="88" t="s">
+      <c r="W21" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="X21" s="89"/>
-      <c r="Y21" s="89"/>
-      <c r="Z21" s="89"/>
-      <c r="AA21" s="89"/>
+      <c r="X21" s="92"/>
+      <c r="Y21" s="92"/>
+      <c r="Z21" s="92"/>
+      <c r="AA21" s="92"/>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B22" s="11" t="s">
@@ -9038,11 +9063,11 @@
       <c r="V22" s="5">
         <v>0</v>
       </c>
-      <c r="W22" s="89"/>
-      <c r="X22" s="89"/>
-      <c r="Y22" s="89"/>
-      <c r="Z22" s="89"/>
-      <c r="AA22" s="89"/>
+      <c r="W22" s="92"/>
+      <c r="X22" s="92"/>
+      <c r="Y22" s="92"/>
+      <c r="Z22" s="92"/>
+      <c r="AA22" s="92"/>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
@@ -9105,11 +9130,11 @@
       <c r="V23" s="5">
         <v>0</v>
       </c>
-      <c r="W23" s="89"/>
-      <c r="X23" s="89"/>
-      <c r="Y23" s="89"/>
-      <c r="Z23" s="89"/>
-      <c r="AA23" s="89"/>
+      <c r="W23" s="92"/>
+      <c r="X23" s="92"/>
+      <c r="Y23" s="92"/>
+      <c r="Z23" s="92"/>
+      <c r="AA23" s="92"/>
     </row>
     <row r="24" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13" t="s">
@@ -9185,13 +9210,13 @@
       <c r="V25" s="17">
         <v>0</v>
       </c>
-      <c r="W25" s="81" t="s">
+      <c r="W25" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="X25" s="81"/>
-      <c r="Y25" s="81"/>
-      <c r="Z25" s="81"/>
-      <c r="AA25" s="81"/>
+      <c r="X25" s="84"/>
+      <c r="Y25" s="84"/>
+      <c r="Z25" s="84"/>
+      <c r="AA25" s="84"/>
     </row>
     <row r="26" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="16" t="s">
@@ -9255,11 +9280,11 @@
       <c r="V26" s="17">
         <v>0</v>
       </c>
-      <c r="W26" s="81"/>
-      <c r="X26" s="81"/>
-      <c r="Y26" s="81"/>
-      <c r="Z26" s="81"/>
-      <c r="AA26" s="81"/>
+      <c r="W26" s="84"/>
+      <c r="X26" s="84"/>
+      <c r="Y26" s="84"/>
+      <c r="Z26" s="84"/>
+      <c r="AA26" s="84"/>
     </row>
     <row r="27" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="16" t="s">
@@ -9323,11 +9348,11 @@
       <c r="V27" s="17">
         <v>0</v>
       </c>
-      <c r="W27" s="81"/>
-      <c r="X27" s="81"/>
-      <c r="Y27" s="81"/>
-      <c r="Z27" s="81"/>
-      <c r="AA27" s="81"/>
+      <c r="W27" s="84"/>
+      <c r="X27" s="84"/>
+      <c r="Y27" s="84"/>
+      <c r="Z27" s="84"/>
+      <c r="AA27" s="84"/>
     </row>
     <row r="28" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="16" t="s">
@@ -9391,11 +9416,11 @@
       <c r="V28" s="17">
         <v>0</v>
       </c>
-      <c r="W28" s="81"/>
-      <c r="X28" s="81"/>
-      <c r="Y28" s="81"/>
-      <c r="Z28" s="81"/>
-      <c r="AA28" s="81"/>
+      <c r="W28" s="84"/>
+      <c r="X28" s="84"/>
+      <c r="Y28" s="84"/>
+      <c r="Z28" s="84"/>
+      <c r="AA28" s="84"/>
     </row>
     <row r="29" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
@@ -9471,13 +9496,13 @@
       <c r="V30" s="17">
         <v>0</v>
       </c>
-      <c r="W30" s="81" t="s">
+      <c r="W30" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="X30" s="81"/>
-      <c r="Y30" s="81"/>
-      <c r="Z30" s="81"/>
-      <c r="AA30" s="81"/>
+      <c r="X30" s="84"/>
+      <c r="Y30" s="84"/>
+      <c r="Z30" s="84"/>
+      <c r="AA30" s="84"/>
     </row>
     <row r="31" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
@@ -9541,11 +9566,11 @@
       <c r="V31" s="17">
         <v>0</v>
       </c>
-      <c r="W31" s="81"/>
-      <c r="X31" s="81"/>
-      <c r="Y31" s="81"/>
-      <c r="Z31" s="81"/>
-      <c r="AA31" s="81"/>
+      <c r="W31" s="84"/>
+      <c r="X31" s="84"/>
+      <c r="Y31" s="84"/>
+      <c r="Z31" s="84"/>
+      <c r="AA31" s="84"/>
     </row>
     <row r="32" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="16" t="s">
@@ -9609,11 +9634,11 @@
       <c r="V32" s="17">
         <v>0</v>
       </c>
-      <c r="W32" s="81"/>
-      <c r="X32" s="81"/>
-      <c r="Y32" s="81"/>
-      <c r="Z32" s="81"/>
-      <c r="AA32" s="81"/>
+      <c r="W32" s="84"/>
+      <c r="X32" s="84"/>
+      <c r="Y32" s="84"/>
+      <c r="Z32" s="84"/>
+      <c r="AA32" s="84"/>
     </row>
     <row r="33" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="16" t="s">
@@ -9677,11 +9702,11 @@
       <c r="V33" s="17">
         <v>0</v>
       </c>
-      <c r="W33" s="81"/>
-      <c r="X33" s="81"/>
-      <c r="Y33" s="81"/>
-      <c r="Z33" s="81"/>
-      <c r="AA33" s="81"/>
+      <c r="W33" s="84"/>
+      <c r="X33" s="84"/>
+      <c r="Y33" s="84"/>
+      <c r="Z33" s="84"/>
+      <c r="AA33" s="84"/>
     </row>
     <row r="34" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B34" s="16" t="s">
@@ -9745,11 +9770,11 @@
       <c r="V34" s="17">
         <v>0</v>
       </c>
-      <c r="W34" s="81"/>
-      <c r="X34" s="81"/>
-      <c r="Y34" s="81"/>
-      <c r="Z34" s="81"/>
-      <c r="AA34" s="81"/>
+      <c r="W34" s="84"/>
+      <c r="X34" s="84"/>
+      <c r="Y34" s="84"/>
+      <c r="Z34" s="84"/>
+      <c r="AA34" s="84"/>
     </row>
     <row r="35" spans="2:27" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="18" t="s">
@@ -10033,13 +10058,13 @@
       <c r="V41" s="25">
         <v>0</v>
       </c>
-      <c r="W41" s="90" t="s">
+      <c r="W41" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="X41" s="90"/>
-      <c r="Y41" s="90"/>
-      <c r="Z41" s="90"/>
-      <c r="AA41" s="90"/>
+      <c r="X41" s="93"/>
+      <c r="Y41" s="93"/>
+      <c r="Z41" s="93"/>
+      <c r="AA41" s="93"/>
     </row>
     <row r="42" spans="2:27" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="23" t="s">
@@ -10087,11 +10112,11 @@
       <c r="V42" s="25">
         <v>0</v>
       </c>
-      <c r="W42" s="90"/>
-      <c r="X42" s="90"/>
-      <c r="Y42" s="90"/>
-      <c r="Z42" s="90"/>
-      <c r="AA42" s="90"/>
+      <c r="W42" s="93"/>
+      <c r="X42" s="93"/>
+      <c r="Y42" s="93"/>
+      <c r="Z42" s="93"/>
+      <c r="AA42" s="93"/>
     </row>
     <row r="43" spans="2:27" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="21" t="s">
@@ -10149,13 +10174,13 @@
       <c r="V44" s="25">
         <v>0</v>
       </c>
-      <c r="W44" s="90" t="s">
+      <c r="W44" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="X44" s="90"/>
-      <c r="Y44" s="90"/>
-      <c r="Z44" s="90"/>
-      <c r="AA44" s="90"/>
+      <c r="X44" s="93"/>
+      <c r="Y44" s="93"/>
+      <c r="Z44" s="93"/>
+      <c r="AA44" s="93"/>
     </row>
     <row r="45" spans="2:27" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B45" s="23" t="s">
@@ -10200,11 +10225,11 @@
       <c r="V45" s="25">
         <v>0</v>
       </c>
-      <c r="W45" s="90"/>
-      <c r="X45" s="90"/>
-      <c r="Y45" s="90"/>
-      <c r="Z45" s="90"/>
-      <c r="AA45" s="90"/>
+      <c r="W45" s="93"/>
+      <c r="X45" s="93"/>
+      <c r="Y45" s="93"/>
+      <c r="Z45" s="93"/>
+      <c r="AA45" s="93"/>
     </row>
     <row r="46" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B46" s="11"/>
@@ -10236,49 +10261,49 @@
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B53" s="84" t="s">
+      <c r="B53" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="C53" s="84"/>
-      <c r="D53" s="84"/>
-      <c r="E53" s="84"/>
-      <c r="F53" s="84"/>
-      <c r="G53" s="84"/>
-      <c r="H53" s="84"/>
-      <c r="I53" s="84"/>
-      <c r="J53" s="84"/>
-      <c r="K53" s="84"/>
-      <c r="L53" s="84"/>
+      <c r="C53" s="87"/>
+      <c r="D53" s="87"/>
+      <c r="E53" s="87"/>
+      <c r="F53" s="87"/>
+      <c r="G53" s="87"/>
+      <c r="H53" s="87"/>
+      <c r="I53" s="87"/>
+      <c r="J53" s="87"/>
+      <c r="K53" s="87"/>
+      <c r="L53" s="87"/>
     </row>
     <row r="54" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="84" t="s">
+      <c r="B54" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C54" s="84"/>
-      <c r="D54" s="84"/>
-      <c r="E54" s="84"/>
-      <c r="F54" s="84"/>
-      <c r="G54" s="84"/>
-      <c r="H54" s="84"/>
-      <c r="I54" s="84"/>
-      <c r="J54" s="84"/>
-      <c r="K54" s="84"/>
-      <c r="L54" s="84"/>
+      <c r="C54" s="87"/>
+      <c r="D54" s="87"/>
+      <c r="E54" s="87"/>
+      <c r="F54" s="87"/>
+      <c r="G54" s="87"/>
+      <c r="H54" s="87"/>
+      <c r="I54" s="87"/>
+      <c r="J54" s="87"/>
+      <c r="K54" s="87"/>
+      <c r="L54" s="87"/>
     </row>
     <row r="55" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="82" t="s">
+      <c r="B55" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="C55" s="82"/>
-      <c r="D55" s="82"/>
-      <c r="E55" s="82"/>
-      <c r="F55" s="82"/>
-      <c r="G55" s="82"/>
-      <c r="H55" s="83"/>
-      <c r="I55" s="83"/>
-      <c r="J55" s="83"/>
-      <c r="K55" s="83"/>
-      <c r="L55" s="83"/>
+      <c r="C55" s="85"/>
+      <c r="D55" s="85"/>
+      <c r="E55" s="85"/>
+      <c r="F55" s="85"/>
+      <c r="G55" s="85"/>
+      <c r="H55" s="86"/>
+      <c r="I55" s="86"/>
+      <c r="J55" s="86"/>
+      <c r="K55" s="86"/>
+      <c r="L55" s="86"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B56" s="28" t="s">
@@ -10306,53 +10331,53 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A2:Z41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:Z45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="53.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
     <col min="3" max="6" width="10.7109375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="86" t="s">
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="87" t="s">
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="87"/>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
-      <c r="V2" s="79" t="s">
+      <c r="R2" s="90"/>
+      <c r="S2" s="90"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="90"/>
+      <c r="V2" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="79"/>
+      <c r="W2" s="82"/>
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -11590,10 +11615,10 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C21" s="2">
-        <v>25</v>
+        <v>690</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -11652,17 +11677,17 @@
       <c r="U21" s="5">
         <v>0</v>
       </c>
-      <c r="V21" s="88" t="s">
+      <c r="V21" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="W21" s="89"/>
-      <c r="X21" s="89"/>
-      <c r="Y21" s="89"/>
-      <c r="Z21" s="89"/>
+      <c r="W21" s="92"/>
+      <c r="X21" s="92"/>
+      <c r="Y21" s="92"/>
+      <c r="Z21" s="92"/>
     </row>
     <row r="22" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>81</v>
+        <v>203</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>85</v>
@@ -11694,11 +11719,11 @@
     </row>
     <row r="23" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="D23" s="15">
         <v>1</v>
@@ -11762,9 +11787,11 @@
     </row>
     <row r="24" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="15"/>
+        <v>204</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>85</v>
+      </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="2"/>
@@ -11792,11 +11819,11 @@
     </row>
     <row r="25" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15">
-        <v>32</v>
+        <v>231</v>
       </c>
       <c r="D25" s="15">
         <v>1</v>
@@ -11858,108 +11885,279 @@
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
+    <row r="26" spans="1:26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="15">
+        <v>888</v>
+      </c>
+      <c r="D27" t="s">
+        <v>202</v>
+      </c>
+      <c r="E27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27" s="81">
+        <f>G23</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="81">
+        <f t="shared" ref="H27:U29" si="0">H23</f>
+        <v>1.292035409950081</v>
+      </c>
+      <c r="I27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="81">
+        <f t="shared" si="0"/>
+        <v>0.21609557903205395</v>
+      </c>
+      <c r="K27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U27" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="15">
+        <v>887</v>
+      </c>
+      <c r="D29" t="s">
+        <v>202</v>
+      </c>
+      <c r="E29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29" s="81">
+        <f>G25</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="81">
+        <f t="shared" si="0"/>
+        <v>8.9861584913475845E-2</v>
+      </c>
+      <c r="I29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="81">
+        <f t="shared" si="0"/>
+        <v>0.77744778478068477</v>
+      </c>
+      <c r="K29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U29" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="80"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="B27" s="77">
+      <c r="B31" s="77">
         <f>1/1.43</f>
         <v>0.69930069930069938</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A32" s="11"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="91" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="91"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="91"/>
-      <c r="H33" s="91"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="91"/>
-      <c r="K33" s="91"/>
-    </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="91" t="s">
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
+      <c r="K37" s="94"/>
+    </row>
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="91"/>
-      <c r="C34" s="91"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="91"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="91"/>
-      <c r="H34" s="91"/>
-      <c r="I34" s="91"/>
-      <c r="J34" s="91"/>
-      <c r="K34" s="91"/>
-    </row>
-    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="83" t="s">
+      <c r="B38" s="94"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="94"/>
+      <c r="I38" s="94"/>
+      <c r="J38" s="94"/>
+      <c r="K38" s="94"/>
+    </row>
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="83"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="83"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83"/>
-      <c r="J35" s="83"/>
-      <c r="K35" s="83"/>
-    </row>
-    <row r="36" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="41" t="s">
+      <c r="B39" s="86"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="86"/>
+      <c r="I39" s="86"/>
+      <c r="J39" s="86"/>
+      <c r="K39" s="86"/>
+    </row>
+    <row r="40" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="B36" s="44"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="B40" s="44"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B37" s="43"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="46" t="s">
+      <c r="B41" s="43"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="46" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="42"/>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:K35"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A39:K39"/>
     <mergeCell ref="V2:Z2"/>
     <mergeCell ref="V21:Z21"/>
-    <mergeCell ref="A33:K33"/>
+    <mergeCell ref="A37:K37"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="L2:P2"/>
     <mergeCell ref="Q2:U2"/>
@@ -11971,20 +12169,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:AP20"/>
+  <dimension ref="A1:AP22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP5" sqref="AP5"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="84.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -12144,8 +12342,8 @@
       <c r="AO1" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="AP1" s="101" t="s">
-        <v>200</v>
+      <c r="AP1" s="79" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
@@ -14838,16 +15036,16 @@
     </row>
     <row r="18" spans="1:42" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="41" t="str">
-        <f>"I-680 Sunol EL SB "&amp;'tolls 2015'!A21</f>
-        <v>I-680 Sunol EL SB Entire length</v>
+        <f>"I-680 Sunol EL SB: "&amp;'tolls 2015'!A21</f>
+        <v>I-680 Sunol EL SB: SCL County Line to SR84</v>
       </c>
       <c r="B18" s="41">
         <f>C18*1000+D18*10+F18</f>
-        <v>25004</v>
+        <v>690004</v>
       </c>
       <c r="C18" s="41">
         <f>'tolls 2015'!C21</f>
-        <v>25</v>
+        <v>690</v>
       </c>
       <c r="D18" s="41">
         <f>'tolls 2015'!D21</f>
@@ -15005,16 +15203,16 @@
     </row>
     <row r="19" spans="1:42" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="41" t="str">
-        <f>"SR-237 EL SB "&amp;'tolls 2015'!A23</f>
-        <v>SR-237 EL SB Entire length</v>
+        <f>"SR-237 EL SB: "&amp;'tolls 2015'!A23</f>
+        <v>SR-237 EL SB: US101 Interchange to I-880 Interchange</v>
       </c>
       <c r="B19" s="41">
         <f t="shared" ref="B19:B20" si="29">C19*1000+D19*10+F19</f>
-        <v>31004</v>
+        <v>232004</v>
       </c>
       <c r="C19" s="41">
         <f>'tolls 2015'!C23</f>
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="D19" s="41">
         <v>0</v>
@@ -15171,16 +15369,16 @@
     </row>
     <row r="20" spans="1:42" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="41" t="str">
-        <f>"SR-237 EL NB "&amp;'tolls 2015'!A25</f>
-        <v>SR-237 EL NB Entire length</v>
+        <f>"SR-237 EL NB: "&amp;'tolls 2015'!A25</f>
+        <v>SR-237 EL NB: US101 Interchange to I-880 Interchange</v>
       </c>
       <c r="B20" s="41">
         <f t="shared" si="29"/>
-        <v>32004</v>
+        <v>231004</v>
       </c>
       <c r="C20" s="41">
         <f>'tolls 2015'!C25</f>
-        <v>32</v>
+        <v>231</v>
       </c>
       <c r="D20" s="41">
         <v>0</v>
@@ -15332,6 +15530,338 @@
         <v>0</v>
       </c>
       <c r="AP20" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="str">
+        <f>CONCATENATE('tolls 2015'!A26, " ",'tolls 2015'!A27)</f>
+        <v>SR-237 Express Lanes (first segment before TOLLCLASS 232): I-880 SCL - SR237 to SR262 Mission Blvd - SB</v>
+      </c>
+      <c r="B21" s="41">
+        <f t="shared" ref="B21" si="30">C21*1000+D21*10+F21</f>
+        <v>888004</v>
+      </c>
+      <c r="C21" s="1">
+        <f>'tolls 2015'!C27</f>
+        <v>888</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" s="41">
+        <v>4</v>
+      </c>
+      <c r="G21" s="39">
+        <f>IF('tolls 2015'!G27="n/a",0,'tolls 2015'!G27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="39">
+        <f>IF('tolls 2015'!H27="n/a",0,'tolls 2015'!H27)*CPI_2015_to_2000</f>
+        <v>0.90352126569935742</v>
+      </c>
+      <c r="I21" s="39">
+        <f>IF('tolls 2015'!I27="n/a",0,'tolls 2015'!I27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="39">
+        <f>IF('tolls 2015'!J27="n/a",0,'tolls 2015'!J27)*CPI_2015_to_2000</f>
+        <v>0.15111578953290489</v>
+      </c>
+      <c r="K21" s="39">
+        <f>IF('tolls 2015'!K27="n/a",0,'tolls 2015'!K27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="39">
+        <f>IF('tolls 2015'!L27="n/a",0,'tolls 2015'!L27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="39">
+        <f>IF('tolls 2015'!M27="n/a",0,'tolls 2015'!M27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="39">
+        <f>IF('tolls 2015'!N27="n/a",0,'tolls 2015'!N27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="39">
+        <f>IF('tolls 2015'!O27="n/a",0,'tolls 2015'!O27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="39">
+        <f>IF('tolls 2015'!P27="n/a",0,'tolls 2015'!P27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="39">
+        <f>IF('tolls 2015'!Q27="n/a",0,'tolls 2015'!Q27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="39">
+        <f>IF('tolls 2015'!R27="n/a",0,'tolls 2015'!R27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="39">
+        <f>IF('tolls 2015'!S27="n/a",0,'tolls 2015'!S27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="39">
+        <f>IF('tolls 2015'!T27="n/a",0,'tolls 2015'!T27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="U21" s="39">
+        <f>IF('tolls 2015'!U27="n/a",0,'tolls 2015'!U27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="V21" s="39">
+        <f>IF('tolls 2015'!G27="n/a",0,'tolls 2015'!G27)</f>
+        <v>0</v>
+      </c>
+      <c r="W21" s="39">
+        <f>IF('tolls 2015'!H27="n/a",0,'tolls 2015'!H27)</f>
+        <v>1.292035409950081</v>
+      </c>
+      <c r="X21" s="39">
+        <f>IF('tolls 2015'!I27="n/a",0,'tolls 2015'!I27)</f>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="39">
+        <f>IF('tolls 2015'!J27="n/a",0,'tolls 2015'!J27)</f>
+        <v>0.21609557903205395</v>
+      </c>
+      <c r="Z21" s="39">
+        <f>IF('tolls 2015'!K27="n/a",0,'tolls 2015'!K27)</f>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="39">
+        <f>IF('tolls 2015'!G27="n/a",0,'tolls 2015'!G27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="39">
+        <f>IF('tolls 2015'!H27="n/a",0,'tolls 2015'!H27)*CPI_2015_to_2000</f>
+        <v>0.90352126569935742</v>
+      </c>
+      <c r="AC21" s="39">
+        <f>IF('tolls 2015'!I27="n/a",0,'tolls 2015'!I27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="39">
+        <f>IF('tolls 2015'!J27="n/a",0,'tolls 2015'!J27)*CPI_2015_to_2000</f>
+        <v>0.15111578953290489</v>
+      </c>
+      <c r="AE21" s="39">
+        <f>IF('tolls 2015'!K27="n/a",0,'tolls 2015'!K27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AF21" s="39">
+        <f>IF('tolls 2015'!G27="n/a",0,'tolls 2015'!G27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AG21" s="39">
+        <f>IF('tolls 2015'!H27="n/a",0,'tolls 2015'!H27)*CPI_2015_to_2000</f>
+        <v>0.90352126569935742</v>
+      </c>
+      <c r="AH21" s="39">
+        <f>IF('tolls 2015'!I27="n/a",0,'tolls 2015'!I27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AI21" s="39">
+        <f>IF('tolls 2015'!J27="n/a",0,'tolls 2015'!J27)*CPI_2015_to_2000</f>
+        <v>0.15111578953290489</v>
+      </c>
+      <c r="AJ21" s="39">
+        <f>IF('tolls 2015'!K27="n/a",0,'tolls 2015'!K27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AK21" s="39">
+        <f>IF('tolls 2015'!G27="n/a",0,'tolls 2015'!G27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AL21" s="39">
+        <f>IF('tolls 2015'!H27="n/a",0,'tolls 2015'!H27)*CPI_2015_to_2000</f>
+        <v>0.90352126569935742</v>
+      </c>
+      <c r="AM21" s="39">
+        <f>IF('tolls 2015'!I27="n/a",0,'tolls 2015'!I27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AN21" s="39">
+        <f>IF('tolls 2015'!J27="n/a",0,'tolls 2015'!J27)*CPI_2015_to_2000</f>
+        <v>0.15111578953290489</v>
+      </c>
+      <c r="AO21" s="39">
+        <f>IF('tolls 2015'!K27="n/a",0,'tolls 2015'!K27)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AP21" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="str">
+        <f>CONCATENATE('tolls 2015'!A28, " ",'tolls 2015'!A29)</f>
+        <v>SR-237 Express Lanes (last segment after TOLLCLASS 231): I-880 SCL - SR237 to SR262 Mission Blvd - NB</v>
+      </c>
+      <c r="B22" s="41">
+        <f t="shared" ref="B22" si="31">C22*1000+D22*10+F22</f>
+        <v>887004</v>
+      </c>
+      <c r="C22" s="1">
+        <f>'tolls 2015'!C29</f>
+        <v>887</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="F22" s="41">
+        <v>4</v>
+      </c>
+      <c r="G22" s="39">
+        <f>IF('tolls 2015'!G29="n/a",0,'tolls 2015'!G29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="39">
+        <f>IF('tolls 2015'!H29="n/a",0,'tolls 2015'!H29)*CPI_2015_to_2000</f>
+        <v>6.2840269170262836E-2</v>
+      </c>
+      <c r="I22" s="39">
+        <f>IF('tolls 2015'!I29="n/a",0,'tolls 2015'!I29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="39">
+        <f>IF('tolls 2015'!J29="n/a",0,'tolls 2015'!J29)*CPI_2015_to_2000</f>
+        <v>0.54366977956691254</v>
+      </c>
+      <c r="K22" s="39">
+        <f>IF('tolls 2015'!K29="n/a",0,'tolls 2015'!K29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="L22" s="39">
+        <f>IF('tolls 2015'!L29="n/a",0,'tolls 2015'!L29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="39">
+        <f>IF('tolls 2015'!M29="n/a",0,'tolls 2015'!M29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="39">
+        <f>IF('tolls 2015'!N29="n/a",0,'tolls 2015'!N29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="39">
+        <f>IF('tolls 2015'!O29="n/a",0,'tolls 2015'!O29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="39">
+        <f>IF('tolls 2015'!P29="n/a",0,'tolls 2015'!P29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="39">
+        <f>IF('tolls 2015'!Q29="n/a",0,'tolls 2015'!Q29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="39">
+        <f>IF('tolls 2015'!R29="n/a",0,'tolls 2015'!R29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="39">
+        <f>IF('tolls 2015'!S29="n/a",0,'tolls 2015'!S29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="39">
+        <f>IF('tolls 2015'!T29="n/a",0,'tolls 2015'!T29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="39">
+        <f>IF('tolls 2015'!U29="n/a",0,'tolls 2015'!U29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="V22" s="39">
+        <f>IF('tolls 2015'!G29="n/a",0,'tolls 2015'!G29)</f>
+        <v>0</v>
+      </c>
+      <c r="W22" s="39">
+        <f>IF('tolls 2015'!H29="n/a",0,'tolls 2015'!H29)</f>
+        <v>8.9861584913475845E-2</v>
+      </c>
+      <c r="X22" s="39">
+        <f>IF('tolls 2015'!I29="n/a",0,'tolls 2015'!I29)</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="39">
+        <f>IF('tolls 2015'!J29="n/a",0,'tolls 2015'!J29)</f>
+        <v>0.77744778478068477</v>
+      </c>
+      <c r="Z22" s="39">
+        <f>IF('tolls 2015'!K29="n/a",0,'tolls 2015'!K29)</f>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="39">
+        <f>IF('tolls 2015'!G29="n/a",0,'tolls 2015'!G29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="39">
+        <f>IF('tolls 2015'!H29="n/a",0,'tolls 2015'!H29)*CPI_2015_to_2000</f>
+        <v>6.2840269170262836E-2</v>
+      </c>
+      <c r="AC22" s="39">
+        <f>IF('tolls 2015'!I29="n/a",0,'tolls 2015'!I29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="39">
+        <f>IF('tolls 2015'!J29="n/a",0,'tolls 2015'!J29)*CPI_2015_to_2000</f>
+        <v>0.54366977956691254</v>
+      </c>
+      <c r="AE22" s="39">
+        <f>IF('tolls 2015'!K29="n/a",0,'tolls 2015'!K29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="39">
+        <f>IF('tolls 2015'!G29="n/a",0,'tolls 2015'!G29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AG22" s="39">
+        <f>IF('tolls 2015'!H29="n/a",0,'tolls 2015'!H29)*CPI_2015_to_2000</f>
+        <v>6.2840269170262836E-2</v>
+      </c>
+      <c r="AH22" s="39">
+        <f>IF('tolls 2015'!I29="n/a",0,'tolls 2015'!I29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AI22" s="39">
+        <f>IF('tolls 2015'!J29="n/a",0,'tolls 2015'!J29)*CPI_2015_to_2000</f>
+        <v>0.54366977956691254</v>
+      </c>
+      <c r="AJ22" s="39">
+        <f>IF('tolls 2015'!K29="n/a",0,'tolls 2015'!K29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AK22" s="39">
+        <f>IF('tolls 2015'!G29="n/a",0,'tolls 2015'!G29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AL22" s="39">
+        <f>IF('tolls 2015'!H29="n/a",0,'tolls 2015'!H29)*CPI_2015_to_2000</f>
+        <v>6.2840269170262836E-2</v>
+      </c>
+      <c r="AM22" s="39">
+        <f>IF('tolls 2015'!I29="n/a",0,'tolls 2015'!I29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AN22" s="39">
+        <f>IF('tolls 2015'!J29="n/a",0,'tolls 2015'!J29)*CPI_2015_to_2000</f>
+        <v>0.54366977956691254</v>
+      </c>
+      <c r="AO22" s="39">
+        <f>IF('tolls 2015'!K29="n/a",0,'tolls 2015'!K29)*CPI_2015_to_2000</f>
+        <v>0</v>
+      </c>
+      <c r="AP22" s="41">
         <v>0</v>
       </c>
     </row>
@@ -15342,7 +15872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
@@ -18158,15 +18688,15 @@
     <row r="18" spans="1:41" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="str">
         <f>"I-680 SEL SB "&amp;'tolls 2015'!A21</f>
-        <v>I-680 SEL SB Entire length</v>
+        <v>I-680 SEL SB SCL County Line to SR84</v>
       </c>
       <c r="B18" s="29">
         <f>C18*1000+D18*10+F18</f>
-        <v>25004</v>
+        <v>690004</v>
       </c>
       <c r="C18" s="29">
         <f>'tolls 2015'!C21</f>
-        <v>25</v>
+        <v>690</v>
       </c>
       <c r="D18" s="29">
         <f>'tolls 2015'!D21</f>
@@ -20138,15 +20668,15 @@
     <row r="30" spans="1:41" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="str">
         <f>"SR-237 EL SB "&amp;'tolls 2015'!A23</f>
-        <v>SR-237 EL SB Entire length</v>
+        <v>SR-237 EL SB US101 Interchange to I-880 Interchange</v>
       </c>
       <c r="B30" s="31">
         <f t="shared" si="17"/>
-        <v>31014</v>
+        <v>232014</v>
       </c>
       <c r="C30" s="31">
         <f>'tolls 2015'!C23</f>
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="D30" s="31">
         <f>'tolls 2015'!D23</f>
@@ -20303,15 +20833,15 @@
     <row r="31" spans="1:41" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="str">
         <f>"SR-237 EL NB "&amp;'tolls 2015'!A25</f>
-        <v>SR-237 EL NB Entire length</v>
+        <v>SR-237 EL NB US101 Interchange to I-880 Interchange</v>
       </c>
       <c r="B31" s="31">
         <f t="shared" si="17"/>
-        <v>32014</v>
+        <v>231014</v>
       </c>
       <c r="C31" s="31">
         <f>'tolls 2015'!C25</f>
-        <v>32</v>
+        <v>231</v>
       </c>
       <c r="D31" s="31">
         <f>'tolls 2015'!D25</f>
@@ -21051,7 +21581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21077,7 +21607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21114,7 +21644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Set da/sr2 tolls to match their GP counterparts on bridge HOV links
For when these links open to GP during off-peak times
</commit_message>
<xml_diff>
--- a/hwy/Tolls_TM1.5.xlsx
+++ b/hwy/Tolls_TM1.5.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\Networks\TM1_2015_Base_Network\hwy\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D5821C-5415-44C2-A82D-6380F393C617}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="2040" windowWidth="26205" windowHeight="11565" tabRatio="858" activeTab="4"/>
+    <workbookView xWindow="2745" yWindow="1020" windowWidth="26640" windowHeight="12825" tabRatio="858" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" tolls 2010 NOT USED" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
     <definedName name="CPI_2015_to_2000">'tolls 2015'!$B$31</definedName>
     <definedName name="CPI_2015_to_2010" localSheetId="2">'tolls 2015 (wsp) NOT USED'!$C$47</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,12 +46,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Flavia Tsang</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -127,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="209">
   <si>
     <t>TollBooth</t>
   </si>
@@ -953,7 +954,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -1239,7 +1240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1336,12 +1337,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1570,6 +1589,24 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1608,7 +1645,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1674,7 +1711,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1729,7 +1766,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EC9DBF03-1652-45AC-BAE5-60A830A343AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC9DBF03-1652-45AC-BAE5-60A830A343AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1777,7 +1814,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8543A9F4-5207-4914-A667-5ACB39771DFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8543A9F4-5207-4914-A667-5ACB39771DFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1825,7 +1862,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3FB7EF22-B7FB-42C2-B140-4D5A64BAB2EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB7EF22-B7FB-42C2-B140-4D5A64BAB2EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2149,7 +2186,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3736,7 +3773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B43:K45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3775,7 +3812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B42"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -3796,7 +3833,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
@@ -4365,7 +4402,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
@@ -7650,7 +7687,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10331,14 +10368,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:Z45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="A19" sqref="A18:Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10460,1146 +10497,1172 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="104" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="2">
+      <c r="B4" s="105"/>
+      <c r="C4" s="105">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="105">
+        <v>0</v>
+      </c>
+      <c r="E4" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="105">
         <v>1</v>
       </c>
-      <c r="G4" s="5">
-        <v>5</v>
-      </c>
-      <c r="H4" s="5">
-        <v>5</v>
-      </c>
-      <c r="I4" s="5">
-        <v>5</v>
-      </c>
-      <c r="J4" s="5">
-        <v>5</v>
-      </c>
-      <c r="K4" s="5">
-        <v>5</v>
-      </c>
-      <c r="L4" s="5">
-        <v>5</v>
-      </c>
-      <c r="M4" s="5">
-        <v>5</v>
-      </c>
-      <c r="N4" s="5">
-        <v>5</v>
-      </c>
-      <c r="O4" s="5">
-        <v>5</v>
-      </c>
-      <c r="P4" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>5</v>
-      </c>
-      <c r="R4" s="5">
-        <v>5</v>
-      </c>
-      <c r="S4" s="5">
-        <v>5</v>
-      </c>
-      <c r="T4" s="5">
-        <v>5</v>
-      </c>
-      <c r="U4" s="5">
-        <v>5</v>
-      </c>
-      <c r="V4" s="5">
+      <c r="G4" s="106">
+        <v>5</v>
+      </c>
+      <c r="H4" s="106">
+        <v>5</v>
+      </c>
+      <c r="I4" s="106">
+        <v>5</v>
+      </c>
+      <c r="J4" s="106">
+        <v>5</v>
+      </c>
+      <c r="K4" s="106">
+        <v>5</v>
+      </c>
+      <c r="L4" s="106">
+        <v>5</v>
+      </c>
+      <c r="M4" s="106">
+        <v>5</v>
+      </c>
+      <c r="N4" s="106">
+        <v>5</v>
+      </c>
+      <c r="O4" s="106">
+        <v>5</v>
+      </c>
+      <c r="P4" s="106">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="106">
+        <v>5</v>
+      </c>
+      <c r="R4" s="106">
+        <v>5</v>
+      </c>
+      <c r="S4" s="106">
+        <v>5</v>
+      </c>
+      <c r="T4" s="106">
+        <v>5</v>
+      </c>
+      <c r="U4" s="106">
+        <v>5</v>
+      </c>
+      <c r="V4" s="106">
         <v>15</v>
       </c>
-      <c r="W4" s="5">
+      <c r="W4" s="106">
         <v>20</v>
       </c>
-      <c r="X4" s="5">
+      <c r="X4" s="106">
         <v>25</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Y4" s="106">
         <v>30</v>
       </c>
-      <c r="Z4" s="5">
+      <c r="Z4" s="106">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="2">
+      <c r="B5" s="108"/>
+      <c r="C5" s="108">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="108">
+        <v>0</v>
+      </c>
+      <c r="E5" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="108">
         <v>3</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>5</v>
-      </c>
-      <c r="R5" s="7">
+      <c r="G5" s="109">
+        <v>5</v>
+      </c>
+      <c r="H5" s="109">
+        <v>5</v>
+      </c>
+      <c r="I5" s="109">
+        <v>5</v>
+      </c>
+      <c r="J5" s="109">
+        <v>5</v>
+      </c>
+      <c r="K5" s="109">
+        <v>5</v>
+      </c>
+      <c r="L5" s="109">
+        <v>5</v>
+      </c>
+      <c r="M5" s="109">
+        <v>5</v>
+      </c>
+      <c r="N5" s="109">
+        <v>5</v>
+      </c>
+      <c r="O5" s="109">
+        <v>5</v>
+      </c>
+      <c r="P5" s="109">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="109">
+        <v>5</v>
+      </c>
+      <c r="R5" s="110">
         <v>2.5</v>
       </c>
-      <c r="S5" s="5">
-        <v>5</v>
-      </c>
-      <c r="T5" s="7">
+      <c r="S5" s="109">
+        <v>5</v>
+      </c>
+      <c r="T5" s="110">
         <v>2.5</v>
       </c>
-      <c r="U5" s="5">
-        <v>5</v>
-      </c>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
+      <c r="U5" s="109">
+        <v>5</v>
+      </c>
+      <c r="V5" s="109"/>
+      <c r="W5" s="109"/>
+      <c r="X5" s="109"/>
+      <c r="Y5" s="109"/>
+      <c r="Z5" s="109"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="111" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="2">
+      <c r="B6" s="112"/>
+      <c r="C6" s="112">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="112">
+        <v>0</v>
+      </c>
+      <c r="E6" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="112">
         <v>1</v>
       </c>
-      <c r="G6" s="5">
-        <v>5</v>
-      </c>
-      <c r="H6" s="5">
-        <v>5</v>
-      </c>
-      <c r="I6" s="5">
-        <v>5</v>
-      </c>
-      <c r="J6" s="5">
-        <v>5</v>
-      </c>
-      <c r="K6" s="5">
-        <v>5</v>
-      </c>
-      <c r="L6" s="5">
-        <v>5</v>
-      </c>
-      <c r="M6" s="5">
-        <v>5</v>
-      </c>
-      <c r="N6" s="5">
-        <v>5</v>
-      </c>
-      <c r="O6" s="5">
-        <v>5</v>
-      </c>
-      <c r="P6" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>5</v>
-      </c>
-      <c r="R6" s="5">
-        <v>5</v>
-      </c>
-      <c r="S6" s="5">
-        <v>5</v>
-      </c>
-      <c r="T6" s="5">
-        <v>5</v>
-      </c>
-      <c r="U6" s="5">
-        <v>5</v>
-      </c>
-      <c r="V6" s="5">
+      <c r="G6" s="113">
+        <v>5</v>
+      </c>
+      <c r="H6" s="113">
+        <v>5</v>
+      </c>
+      <c r="I6" s="113">
+        <v>5</v>
+      </c>
+      <c r="J6" s="113">
+        <v>5</v>
+      </c>
+      <c r="K6" s="113">
+        <v>5</v>
+      </c>
+      <c r="L6" s="113">
+        <v>5</v>
+      </c>
+      <c r="M6" s="113">
+        <v>5</v>
+      </c>
+      <c r="N6" s="113">
+        <v>5</v>
+      </c>
+      <c r="O6" s="113">
+        <v>5</v>
+      </c>
+      <c r="P6" s="113">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="113">
+        <v>5</v>
+      </c>
+      <c r="R6" s="113">
+        <v>5</v>
+      </c>
+      <c r="S6" s="113">
+        <v>5</v>
+      </c>
+      <c r="T6" s="113">
+        <v>5</v>
+      </c>
+      <c r="U6" s="113">
+        <v>5</v>
+      </c>
+      <c r="V6" s="113">
         <v>15</v>
       </c>
-      <c r="W6" s="5">
+      <c r="W6" s="113">
         <v>20</v>
       </c>
-      <c r="X6" s="5">
+      <c r="X6" s="113">
         <v>25</v>
       </c>
-      <c r="Y6" s="5">
+      <c r="Y6" s="113">
         <v>30</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="Z6" s="113">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="107" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="2">
+      <c r="B7" s="108"/>
+      <c r="C7" s="108">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="108">
+        <v>0</v>
+      </c>
+      <c r="E7" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="108">
         <v>3</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>5</v>
-      </c>
-      <c r="R7" s="7">
+      <c r="G7" s="109">
+        <v>5</v>
+      </c>
+      <c r="H7" s="109">
+        <v>5</v>
+      </c>
+      <c r="I7" s="109">
+        <v>5</v>
+      </c>
+      <c r="J7" s="109">
+        <v>5</v>
+      </c>
+      <c r="K7" s="109">
+        <v>5</v>
+      </c>
+      <c r="L7" s="109">
+        <v>5</v>
+      </c>
+      <c r="M7" s="109">
+        <v>5</v>
+      </c>
+      <c r="N7" s="109">
+        <v>5</v>
+      </c>
+      <c r="O7" s="109">
+        <v>5</v>
+      </c>
+      <c r="P7" s="109">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="109">
+        <v>5</v>
+      </c>
+      <c r="R7" s="110">
         <v>2.5</v>
       </c>
-      <c r="S7" s="5">
-        <v>5</v>
-      </c>
-      <c r="T7" s="7">
+      <c r="S7" s="109">
+        <v>5</v>
+      </c>
+      <c r="T7" s="110">
         <v>2.5</v>
       </c>
-      <c r="U7" s="5">
-        <v>5</v>
-      </c>
+      <c r="U7" s="109">
+        <v>5</v>
+      </c>
+      <c r="V7" s="107"/>
+      <c r="W7" s="107"/>
+      <c r="X7" s="107"/>
+      <c r="Y7" s="107"/>
+      <c r="Z7" s="107"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="111" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="2">
+      <c r="B8" s="112"/>
+      <c r="C8" s="112">
         <v>8</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="112">
+        <v>0</v>
+      </c>
+      <c r="E8" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="112">
         <v>1</v>
       </c>
-      <c r="G8" s="5">
-        <v>5</v>
-      </c>
-      <c r="H8" s="5">
-        <v>5</v>
-      </c>
-      <c r="I8" s="5">
-        <v>5</v>
-      </c>
-      <c r="J8" s="5">
-        <v>5</v>
-      </c>
-      <c r="K8" s="5">
-        <v>5</v>
-      </c>
-      <c r="L8" s="5">
-        <v>5</v>
-      </c>
-      <c r="M8" s="5">
-        <v>5</v>
-      </c>
-      <c r="N8" s="5">
-        <v>5</v>
-      </c>
-      <c r="O8" s="5">
-        <v>5</v>
-      </c>
-      <c r="P8" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>5</v>
-      </c>
-      <c r="R8" s="5">
-        <v>5</v>
-      </c>
-      <c r="S8" s="5">
-        <v>5</v>
-      </c>
-      <c r="T8" s="5">
-        <v>5</v>
-      </c>
-      <c r="U8" s="5">
-        <v>5</v>
-      </c>
-      <c r="V8" s="5">
+      <c r="G8" s="113">
+        <v>5</v>
+      </c>
+      <c r="H8" s="113">
+        <v>5</v>
+      </c>
+      <c r="I8" s="113">
+        <v>5</v>
+      </c>
+      <c r="J8" s="113">
+        <v>5</v>
+      </c>
+      <c r="K8" s="113">
+        <v>5</v>
+      </c>
+      <c r="L8" s="113">
+        <v>5</v>
+      </c>
+      <c r="M8" s="113">
+        <v>5</v>
+      </c>
+      <c r="N8" s="113">
+        <v>5</v>
+      </c>
+      <c r="O8" s="113">
+        <v>5</v>
+      </c>
+      <c r="P8" s="113">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="113">
+        <v>5</v>
+      </c>
+      <c r="R8" s="113">
+        <v>5</v>
+      </c>
+      <c r="S8" s="113">
+        <v>5</v>
+      </c>
+      <c r="T8" s="113">
+        <v>5</v>
+      </c>
+      <c r="U8" s="113">
+        <v>5</v>
+      </c>
+      <c r="V8" s="113">
         <v>6</v>
       </c>
-      <c r="W8" s="5">
+      <c r="W8" s="113">
         <v>8.25</v>
       </c>
-      <c r="X8" s="5">
+      <c r="X8" s="113">
         <v>11.25</v>
       </c>
-      <c r="Y8" s="5">
+      <c r="Y8" s="113">
         <v>12</v>
       </c>
-      <c r="Z8" s="5">
+      <c r="Z8" s="113">
         <v>13.5</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="2">
+      <c r="B9" s="108"/>
+      <c r="C9" s="108">
         <v>8</v>
       </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="108">
+        <v>0</v>
+      </c>
+      <c r="E9" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="108">
         <v>3</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q9" s="5">
-        <v>5</v>
-      </c>
-      <c r="R9" s="7">
+      <c r="G9" s="109">
+        <v>5</v>
+      </c>
+      <c r="H9" s="109">
+        <v>5</v>
+      </c>
+      <c r="I9" s="109">
+        <v>5</v>
+      </c>
+      <c r="J9" s="109">
+        <v>5</v>
+      </c>
+      <c r="K9" s="109">
+        <v>5</v>
+      </c>
+      <c r="L9" s="109">
+        <v>5</v>
+      </c>
+      <c r="M9" s="109">
+        <v>5</v>
+      </c>
+      <c r="N9" s="109">
+        <v>5</v>
+      </c>
+      <c r="O9" s="109">
+        <v>5</v>
+      </c>
+      <c r="P9" s="109">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="109">
+        <v>5</v>
+      </c>
+      <c r="R9" s="110">
         <v>2.5</v>
       </c>
-      <c r="S9" s="5">
-        <v>5</v>
-      </c>
-      <c r="T9" s="7">
+      <c r="S9" s="109">
+        <v>5</v>
+      </c>
+      <c r="T9" s="110">
         <v>2.5</v>
       </c>
-      <c r="U9" s="5">
-        <v>5</v>
-      </c>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
+      <c r="U9" s="109">
+        <v>5</v>
+      </c>
+      <c r="V9" s="109"/>
+      <c r="W9" s="109"/>
+      <c r="X9" s="109"/>
+      <c r="Y9" s="109"/>
+      <c r="Z9" s="109"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="111" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="2">
+      <c r="B10" s="112"/>
+      <c r="C10" s="112">
         <v>3</v>
       </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="112">
+        <v>0</v>
+      </c>
+      <c r="E10" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="112">
         <v>1</v>
       </c>
-      <c r="G10" s="5">
-        <v>5</v>
-      </c>
-      <c r="H10" s="5">
-        <v>5</v>
-      </c>
-      <c r="I10" s="5">
-        <v>5</v>
-      </c>
-      <c r="J10" s="5">
-        <v>5</v>
-      </c>
-      <c r="K10" s="5">
-        <v>5</v>
-      </c>
-      <c r="L10" s="5">
-        <v>5</v>
-      </c>
-      <c r="M10" s="5">
-        <v>5</v>
-      </c>
-      <c r="N10" s="5">
-        <v>5</v>
-      </c>
-      <c r="O10" s="5">
-        <v>5</v>
-      </c>
-      <c r="P10" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>5</v>
-      </c>
-      <c r="R10" s="5">
-        <v>5</v>
-      </c>
-      <c r="S10" s="5">
-        <v>5</v>
-      </c>
-      <c r="T10" s="5">
-        <v>5</v>
-      </c>
-      <c r="U10" s="5">
-        <v>5</v>
-      </c>
-      <c r="V10" s="5">
+      <c r="G10" s="113">
+        <v>5</v>
+      </c>
+      <c r="H10" s="113">
+        <v>5</v>
+      </c>
+      <c r="I10" s="113">
+        <v>5</v>
+      </c>
+      <c r="J10" s="113">
+        <v>5</v>
+      </c>
+      <c r="K10" s="113">
+        <v>5</v>
+      </c>
+      <c r="L10" s="113">
+        <v>5</v>
+      </c>
+      <c r="M10" s="113">
+        <v>5</v>
+      </c>
+      <c r="N10" s="113">
+        <v>5</v>
+      </c>
+      <c r="O10" s="113">
+        <v>5</v>
+      </c>
+      <c r="P10" s="113">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="113">
+        <v>5</v>
+      </c>
+      <c r="R10" s="113">
+        <v>5</v>
+      </c>
+      <c r="S10" s="113">
+        <v>5</v>
+      </c>
+      <c r="T10" s="113">
+        <v>5</v>
+      </c>
+      <c r="U10" s="113">
+        <v>5</v>
+      </c>
+      <c r="V10" s="113">
         <v>15</v>
       </c>
-      <c r="W10" s="5">
+      <c r="W10" s="113">
         <v>20</v>
       </c>
-      <c r="X10" s="5">
+      <c r="X10" s="113">
         <v>25</v>
       </c>
-      <c r="Y10" s="5">
+      <c r="Y10" s="113">
         <v>30</v>
       </c>
-      <c r="Z10" s="5">
+      <c r="Z10" s="113">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="2">
+      <c r="B11" s="108"/>
+      <c r="C11" s="108">
         <v>3</v>
       </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="108">
+        <v>0</v>
+      </c>
+      <c r="E11" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="108">
         <v>3</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q11" s="5">
-        <v>5</v>
-      </c>
-      <c r="R11" s="7">
+      <c r="G11" s="109">
+        <v>5</v>
+      </c>
+      <c r="H11" s="109">
+        <v>5</v>
+      </c>
+      <c r="I11" s="109">
+        <v>5</v>
+      </c>
+      <c r="J11" s="109">
+        <v>5</v>
+      </c>
+      <c r="K11" s="109">
+        <v>5</v>
+      </c>
+      <c r="L11" s="109">
+        <v>5</v>
+      </c>
+      <c r="M11" s="109">
+        <v>5</v>
+      </c>
+      <c r="N11" s="109">
+        <v>5</v>
+      </c>
+      <c r="O11" s="109">
+        <v>5</v>
+      </c>
+      <c r="P11" s="109">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="109">
+        <v>5</v>
+      </c>
+      <c r="R11" s="110">
         <v>2.5</v>
       </c>
-      <c r="S11" s="5">
-        <v>5</v>
-      </c>
-      <c r="T11" s="7">
+      <c r="S11" s="109">
+        <v>5</v>
+      </c>
+      <c r="T11" s="110">
         <v>2.5</v>
       </c>
-      <c r="U11" s="5">
-        <v>5</v>
-      </c>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
+      <c r="U11" s="109">
+        <v>5</v>
+      </c>
+      <c r="V11" s="109"/>
+      <c r="W11" s="109"/>
+      <c r="X11" s="109"/>
+      <c r="Y11" s="109"/>
+      <c r="Z11" s="109"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="111" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="B12" s="112"/>
+      <c r="C12" s="112">
+        <v>5</v>
+      </c>
+      <c r="D12" s="112">
+        <v>0</v>
+      </c>
+      <c r="E12" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="112">
         <v>1</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="113">
         <v>4</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="113">
         <v>6</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="113">
         <v>4</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="113">
         <v>6</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="113">
         <v>4</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="113">
         <v>4</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="113">
         <v>6</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="113">
         <v>4</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="113">
         <v>6</v>
       </c>
-      <c r="P12" s="5">
+      <c r="P12" s="113">
         <v>4</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="113">
         <v>4</v>
       </c>
-      <c r="R12" s="8">
+      <c r="R12" s="114">
         <v>6</v>
       </c>
-      <c r="S12" s="5">
+      <c r="S12" s="113">
         <v>4</v>
       </c>
-      <c r="T12" s="8">
+      <c r="T12" s="114">
         <v>6</v>
       </c>
-      <c r="U12" s="5">
+      <c r="U12" s="113">
         <v>4</v>
       </c>
-      <c r="V12" s="5">
+      <c r="V12" s="113">
         <v>6</v>
       </c>
-      <c r="W12" s="5">
+      <c r="W12" s="113">
         <v>8.25</v>
       </c>
-      <c r="X12" s="5">
+      <c r="X12" s="113">
         <v>11.25</v>
       </c>
-      <c r="Y12" s="5">
+      <c r="Y12" s="113">
         <v>12</v>
       </c>
-      <c r="Z12" s="5">
+      <c r="Z12" s="113">
         <v>13.5</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="B13" s="108"/>
+      <c r="C13" s="108">
+        <v>5</v>
+      </c>
+      <c r="D13" s="108">
+        <v>0</v>
+      </c>
+      <c r="E13" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="108">
         <v>3</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q13" s="5">
+      <c r="G13" s="109">
         <v>4</v>
       </c>
-      <c r="R13" s="9">
+      <c r="H13" s="109">
+        <v>6</v>
+      </c>
+      <c r="I13" s="109">
+        <v>4</v>
+      </c>
+      <c r="J13" s="109">
+        <v>6</v>
+      </c>
+      <c r="K13" s="109">
+        <v>4</v>
+      </c>
+      <c r="L13" s="109">
+        <v>4</v>
+      </c>
+      <c r="M13" s="109">
+        <v>6</v>
+      </c>
+      <c r="N13" s="109">
+        <v>4</v>
+      </c>
+      <c r="O13" s="109">
+        <v>6</v>
+      </c>
+      <c r="P13" s="109">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="109">
+        <v>4</v>
+      </c>
+      <c r="R13" s="115">
         <v>2.5</v>
       </c>
-      <c r="S13" s="5">
+      <c r="S13" s="109">
         <v>4</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="115">
         <v>2.5</v>
       </c>
-      <c r="U13" s="5">
+      <c r="U13" s="109">
         <v>4</v>
       </c>
+      <c r="V13" s="107"/>
+      <c r="W13" s="107"/>
+      <c r="X13" s="107"/>
+      <c r="Y13" s="107"/>
+      <c r="Z13" s="107"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="111" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="2">
+      <c r="B14" s="112"/>
+      <c r="C14" s="112">
         <v>4</v>
       </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="112">
+        <v>0</v>
+      </c>
+      <c r="E14" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="112">
         <v>1</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="113">
         <v>6.75</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="113">
         <v>6.75</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="113">
         <v>6.75</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="113">
         <v>6.75</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="113">
         <v>6.75</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="113">
         <v>6.75</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="113">
         <v>6.75</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="113">
         <v>6.75</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="113">
         <v>6.75</v>
       </c>
-      <c r="P14" s="5">
+      <c r="P14" s="113">
         <v>6.75</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="Q14" s="113">
         <v>6.75</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="113">
         <v>6.75</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S14" s="113">
         <v>6.75</v>
       </c>
-      <c r="T14" s="5">
+      <c r="T14" s="113">
         <v>6.75</v>
       </c>
-      <c r="U14" s="5">
+      <c r="U14" s="113">
         <v>6.75</v>
       </c>
-      <c r="V14" s="5">
+      <c r="V14" s="113">
         <v>20.25</v>
       </c>
-      <c r="W14" s="5">
+      <c r="W14" s="113">
         <v>27</v>
       </c>
-      <c r="X14" s="5">
+      <c r="X14" s="113">
         <v>33.75</v>
       </c>
-      <c r="Y14" s="5">
+      <c r="Y14" s="113">
         <v>40.5</v>
       </c>
-      <c r="Z14" s="5">
+      <c r="Z14" s="113">
         <v>47.25</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="107" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="2">
+      <c r="B15" s="108"/>
+      <c r="C15" s="108">
         <v>4</v>
       </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="108">
+        <v>0</v>
+      </c>
+      <c r="E15" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="108">
         <v>3</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q15" s="5">
+      <c r="G15" s="109">
         <v>6.75</v>
       </c>
-      <c r="R15" s="7">
+      <c r="H15" s="109">
+        <v>6.75</v>
+      </c>
+      <c r="I15" s="109">
+        <v>6.75</v>
+      </c>
+      <c r="J15" s="109">
+        <v>6.75</v>
+      </c>
+      <c r="K15" s="109">
+        <v>6.75</v>
+      </c>
+      <c r="L15" s="109">
+        <v>6.75</v>
+      </c>
+      <c r="M15" s="109">
+        <v>6.75</v>
+      </c>
+      <c r="N15" s="109">
+        <v>6.75</v>
+      </c>
+      <c r="O15" s="109">
+        <v>6.75</v>
+      </c>
+      <c r="P15" s="109">
+        <v>6.75</v>
+      </c>
+      <c r="Q15" s="109">
+        <v>6.75</v>
+      </c>
+      <c r="R15" s="110">
         <v>4.75</v>
       </c>
-      <c r="S15" s="5">
+      <c r="S15" s="109">
         <v>6.75</v>
       </c>
-      <c r="T15" s="7">
+      <c r="T15" s="110">
         <v>4.75</v>
       </c>
-      <c r="U15" s="5">
+      <c r="U15" s="109">
         <v>6.75</v>
       </c>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
+      <c r="V15" s="109"/>
+      <c r="W15" s="109"/>
+      <c r="X15" s="109"/>
+      <c r="Y15" s="109"/>
+      <c r="Z15" s="109"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="111" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="2">
+      <c r="B16" s="112"/>
+      <c r="C16" s="112">
         <v>6</v>
       </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="112">
+        <v>0</v>
+      </c>
+      <c r="E16" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="112">
         <v>1</v>
       </c>
-      <c r="G16" s="5">
-        <v>5</v>
-      </c>
-      <c r="H16" s="5">
-        <v>5</v>
-      </c>
-      <c r="I16" s="5">
-        <v>5</v>
-      </c>
-      <c r="J16" s="5">
-        <v>5</v>
-      </c>
-      <c r="K16" s="5">
-        <v>5</v>
-      </c>
-      <c r="L16" s="5">
-        <v>5</v>
-      </c>
-      <c r="M16" s="5">
-        <v>5</v>
-      </c>
-      <c r="N16" s="5">
-        <v>5</v>
-      </c>
-      <c r="O16" s="5">
-        <v>5</v>
-      </c>
-      <c r="P16" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>5</v>
-      </c>
-      <c r="R16" s="5">
-        <v>5</v>
-      </c>
-      <c r="S16" s="5">
-        <v>5</v>
-      </c>
-      <c r="T16" s="5">
-        <v>5</v>
-      </c>
-      <c r="U16" s="5">
-        <v>5</v>
-      </c>
-      <c r="V16" s="5">
+      <c r="G16" s="113">
+        <v>5</v>
+      </c>
+      <c r="H16" s="113">
+        <v>5</v>
+      </c>
+      <c r="I16" s="113">
+        <v>5</v>
+      </c>
+      <c r="J16" s="113">
+        <v>5</v>
+      </c>
+      <c r="K16" s="113">
+        <v>5</v>
+      </c>
+      <c r="L16" s="113">
+        <v>5</v>
+      </c>
+      <c r="M16" s="113">
+        <v>5</v>
+      </c>
+      <c r="N16" s="113">
+        <v>5</v>
+      </c>
+      <c r="O16" s="113">
+        <v>5</v>
+      </c>
+      <c r="P16" s="113">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="113">
+        <v>5</v>
+      </c>
+      <c r="R16" s="113">
+        <v>5</v>
+      </c>
+      <c r="S16" s="113">
+        <v>5</v>
+      </c>
+      <c r="T16" s="113">
+        <v>5</v>
+      </c>
+      <c r="U16" s="113">
+        <v>5</v>
+      </c>
+      <c r="V16" s="113">
         <v>15</v>
       </c>
-      <c r="W16" s="5">
+      <c r="W16" s="113">
         <v>20</v>
       </c>
-      <c r="X16" s="5">
+      <c r="X16" s="113">
         <v>25</v>
       </c>
-      <c r="Y16" s="5">
+      <c r="Y16" s="113">
         <v>30</v>
       </c>
-      <c r="Z16" s="5">
+      <c r="Z16" s="113">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="107" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="2">
+      <c r="B17" s="108"/>
+      <c r="C17" s="108">
         <v>6</v>
       </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="108">
+        <v>0</v>
+      </c>
+      <c r="E17" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="108">
         <v>2</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L17" s="5">
-        <v>5</v>
-      </c>
-      <c r="M17" s="7">
+      <c r="G17" s="109">
+        <v>5</v>
+      </c>
+      <c r="H17" s="109">
+        <v>5</v>
+      </c>
+      <c r="I17" s="109">
+        <v>5</v>
+      </c>
+      <c r="J17" s="109">
+        <v>5</v>
+      </c>
+      <c r="K17" s="109">
+        <v>5</v>
+      </c>
+      <c r="L17" s="109">
+        <v>5</v>
+      </c>
+      <c r="M17" s="110">
         <v>2.5</v>
       </c>
-      <c r="N17" s="5">
-        <v>5</v>
-      </c>
-      <c r="O17" s="7">
+      <c r="N17" s="109">
+        <v>5</v>
+      </c>
+      <c r="O17" s="110">
         <v>2.5</v>
       </c>
-      <c r="P17" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q17" s="5">
-        <v>5</v>
-      </c>
-      <c r="R17" s="7">
+      <c r="P17" s="109">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="109">
+        <v>5</v>
+      </c>
+      <c r="R17" s="110">
         <v>2.5</v>
       </c>
-      <c r="S17" s="5">
-        <v>5</v>
-      </c>
-      <c r="T17" s="7">
+      <c r="S17" s="109">
+        <v>5</v>
+      </c>
+      <c r="T17" s="110">
         <v>2.5</v>
       </c>
-      <c r="U17" s="5">
-        <v>5</v>
-      </c>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
+      <c r="U17" s="109">
+        <v>5</v>
+      </c>
+      <c r="V17" s="109"/>
+      <c r="W17" s="109"/>
+      <c r="X17" s="109"/>
+      <c r="Y17" s="109"/>
+      <c r="Z17" s="109"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="111" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="2">
+      <c r="B18" s="112"/>
+      <c r="C18" s="112">
         <v>7</v>
       </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="112">
+        <v>0</v>
+      </c>
+      <c r="E18" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="112">
         <v>1</v>
       </c>
-      <c r="G18" s="5">
-        <v>5</v>
-      </c>
-      <c r="H18" s="5">
-        <v>5</v>
-      </c>
-      <c r="I18" s="5">
-        <v>5</v>
-      </c>
-      <c r="J18" s="5">
-        <v>5</v>
-      </c>
-      <c r="K18" s="5">
-        <v>5</v>
-      </c>
-      <c r="L18" s="5">
-        <v>5</v>
-      </c>
-      <c r="M18" s="5">
-        <v>5</v>
-      </c>
-      <c r="N18" s="5">
-        <v>5</v>
-      </c>
-      <c r="O18" s="5">
-        <v>5</v>
-      </c>
-      <c r="P18" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q18" s="5">
-        <v>5</v>
-      </c>
-      <c r="R18" s="5">
-        <v>5</v>
-      </c>
-      <c r="S18" s="5">
-        <v>5</v>
-      </c>
-      <c r="T18" s="5">
-        <v>5</v>
-      </c>
-      <c r="U18" s="5">
-        <v>5</v>
-      </c>
-      <c r="V18" s="5">
+      <c r="G18" s="113">
+        <v>5</v>
+      </c>
+      <c r="H18" s="113">
+        <v>5</v>
+      </c>
+      <c r="I18" s="113">
+        <v>5</v>
+      </c>
+      <c r="J18" s="113">
+        <v>5</v>
+      </c>
+      <c r="K18" s="113">
+        <v>5</v>
+      </c>
+      <c r="L18" s="113">
+        <v>5</v>
+      </c>
+      <c r="M18" s="113">
+        <v>5</v>
+      </c>
+      <c r="N18" s="113">
+        <v>5</v>
+      </c>
+      <c r="O18" s="113">
+        <v>5</v>
+      </c>
+      <c r="P18" s="113">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="113">
+        <v>5</v>
+      </c>
+      <c r="R18" s="113">
+        <v>5</v>
+      </c>
+      <c r="S18" s="113">
+        <v>5</v>
+      </c>
+      <c r="T18" s="113">
+        <v>5</v>
+      </c>
+      <c r="U18" s="113">
+        <v>5</v>
+      </c>
+      <c r="V18" s="113">
         <v>15</v>
       </c>
-      <c r="W18" s="5">
+      <c r="W18" s="113">
         <v>20</v>
       </c>
-      <c r="X18" s="5">
+      <c r="X18" s="113">
         <v>25</v>
       </c>
-      <c r="Y18" s="5">
+      <c r="Y18" s="113">
         <v>30</v>
       </c>
-      <c r="Z18" s="5">
+      <c r="Z18" s="113">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="107" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="2">
+      <c r="B19" s="108"/>
+      <c r="C19" s="108">
         <v>7</v>
       </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="108">
+        <v>0</v>
+      </c>
+      <c r="E19" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="108">
         <v>2</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L19" s="5">
-        <v>5</v>
-      </c>
-      <c r="M19" s="7">
+      <c r="G19" s="109">
+        <v>5</v>
+      </c>
+      <c r="H19" s="109">
+        <v>5</v>
+      </c>
+      <c r="I19" s="109">
+        <v>5</v>
+      </c>
+      <c r="J19" s="109">
+        <v>5</v>
+      </c>
+      <c r="K19" s="109">
+        <v>5</v>
+      </c>
+      <c r="L19" s="109">
+        <v>5</v>
+      </c>
+      <c r="M19" s="110">
         <v>2.5</v>
       </c>
-      <c r="N19" s="5">
-        <v>5</v>
-      </c>
-      <c r="O19" s="7">
+      <c r="N19" s="109">
+        <v>5</v>
+      </c>
+      <c r="O19" s="110">
         <v>2.5</v>
       </c>
-      <c r="P19" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q19" s="5">
-        <v>5</v>
-      </c>
-      <c r="R19" s="7">
+      <c r="P19" s="109">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="109">
+        <v>5</v>
+      </c>
+      <c r="R19" s="110">
         <v>2.5</v>
       </c>
-      <c r="S19" s="5">
-        <v>5</v>
-      </c>
-      <c r="T19" s="7">
+      <c r="S19" s="109">
+        <v>5</v>
+      </c>
+      <c r="T19" s="110">
         <v>2.5</v>
       </c>
-      <c r="U19" s="5">
-        <v>5</v>
-      </c>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
-      <c r="Y19" s="5"/>
-      <c r="Z19" s="5"/>
+      <c r="U19" s="109">
+        <v>5</v>
+      </c>
+      <c r="V19" s="109"/>
+      <c r="W19" s="109"/>
+      <c r="X19" s="109"/>
+      <c r="Y19" s="109"/>
+      <c r="Z19" s="109"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -12169,7 +12232,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
@@ -12177,7 +12240,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12540,43 +12603,43 @@
       </c>
       <c r="G3" s="5">
         <f>IF('tolls 2015'!G5="n/a",0,'tolls 2015'!G5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H3" s="5">
         <f>IF('tolls 2015'!H5="n/a",0,'tolls 2015'!H5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I3" s="5">
         <f>IF('tolls 2015'!I5="n/a",0,'tolls 2015'!I5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J3" s="5">
         <f>IF('tolls 2015'!J5="n/a",0,'tolls 2015'!J5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K3" s="5">
         <f>IF('tolls 2015'!K5="n/a",0,'tolls 2015'!K5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L3" s="5">
         <f>IF('tolls 2015'!L5="n/a",0,'tolls 2015'!L5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="M3" s="5">
         <f>IF('tolls 2015'!M5="n/a",0,'tolls 2015'!M5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="N3" s="5">
         <f>IF('tolls 2015'!N5="n/a",0,'tolls 2015'!N5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="O3" s="5">
         <f>IF('tolls 2015'!O5="n/a",0,'tolls 2015'!O5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="P3" s="5">
         <f>IF('tolls 2015'!P5="n/a",0,'tolls 2015'!P5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="Q3" s="5">
         <f>IF('tolls 2015'!Q5="n/a",0,'tolls 2015'!Q5)*CPI_2015_to_2000</f>
@@ -12600,43 +12663,43 @@
       </c>
       <c r="V3" s="5">
         <f>IF('tolls 2015'!G5="n/a",0,'tolls 2015'!G5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W3" s="5">
         <f t="shared" ref="W3:W17" si="1">V3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X3" s="5">
         <f t="shared" ref="X3:X17" si="2">V3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y3" s="5">
         <f t="shared" ref="Y3:Y17" si="3">V3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="5">
         <f t="shared" ref="Z3:Z17" si="4">V3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA3" s="5">
         <f>IF('tolls 2015'!G5="n/a",0,'tolls 2015'!G5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB3" s="5">
         <f t="shared" ref="AB3:AB16" si="5">AA3</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC3" s="5">
         <f t="shared" ref="AC3:AC16" si="6">AA3</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD3" s="5">
         <f t="shared" ref="AD3:AD16" si="7">AA3</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE3" s="5">
         <f t="shared" ref="AE3:AE16" si="8">AA3</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF3" s="5">
         <f>IF('tolls 2015'!V5="n/a",0,'tolls 2015'!V5)*CPI_2015_to_2000</f>
@@ -12876,43 +12939,43 @@
       </c>
       <c r="G5" s="5">
         <f>IF('tolls 2015'!G7="n/a",0,'tolls 2015'!G7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H5" s="5">
         <f>IF('tolls 2015'!H7="n/a",0,'tolls 2015'!H7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I5" s="5">
         <f>IF('tolls 2015'!I7="n/a",0,'tolls 2015'!I7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J5" s="5">
         <f>IF('tolls 2015'!J7="n/a",0,'tolls 2015'!J7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K5" s="5">
         <f>IF('tolls 2015'!K7="n/a",0,'tolls 2015'!K7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L5" s="5">
         <f>IF('tolls 2015'!L7="n/a",0,'tolls 2015'!L7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="M5" s="5">
         <f>IF('tolls 2015'!M7="n/a",0,'tolls 2015'!M7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="N5" s="5">
         <f>IF('tolls 2015'!N7="n/a",0,'tolls 2015'!N7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="O5" s="5">
         <f>IF('tolls 2015'!O7="n/a",0,'tolls 2015'!O7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="P5" s="5">
         <f>IF('tolls 2015'!P7="n/a",0,'tolls 2015'!P7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="Q5" s="5">
         <f>IF('tolls 2015'!Q7="n/a",0,'tolls 2015'!Q7)*CPI_2015_to_2000</f>
@@ -12936,43 +12999,43 @@
       </c>
       <c r="V5" s="5">
         <f>IF('tolls 2015'!G7="n/a",0,'tolls 2015'!G7)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W5" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X5" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y5" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z5" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA5" s="5">
         <f>IF('tolls 2015'!G7="n/a",0,'tolls 2015'!G7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB5" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC5" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD5" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE5" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF5" s="5">
         <f>IF('tolls 2015'!V7="n/a",0,'tolls 2015'!V7)*CPI_2015_to_2000</f>
@@ -13212,43 +13275,43 @@
       </c>
       <c r="G7" s="5">
         <f>IF('tolls 2015'!G9="n/a",0,'tolls 2015'!G9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H7" s="5">
         <f>IF('tolls 2015'!H9="n/a",0,'tolls 2015'!H9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I7" s="5">
         <f>IF('tolls 2015'!I9="n/a",0,'tolls 2015'!I9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J7" s="5">
         <f>IF('tolls 2015'!J9="n/a",0,'tolls 2015'!J9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K7" s="5">
         <f>IF('tolls 2015'!K9="n/a",0,'tolls 2015'!K9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L7" s="5">
         <f>IF('tolls 2015'!L9="n/a",0,'tolls 2015'!L9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="M7" s="5">
         <f>IF('tolls 2015'!M9="n/a",0,'tolls 2015'!M9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="N7" s="5">
         <f>IF('tolls 2015'!N9="n/a",0,'tolls 2015'!N9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="O7" s="5">
         <f>IF('tolls 2015'!O9="n/a",0,'tolls 2015'!O9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="P7" s="5">
         <f>IF('tolls 2015'!P9="n/a",0,'tolls 2015'!P9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="Q7" s="5">
         <f>IF('tolls 2015'!Q9="n/a",0,'tolls 2015'!Q9)*CPI_2015_to_2000</f>
@@ -13272,43 +13335,43 @@
       </c>
       <c r="V7" s="5">
         <f>IF('tolls 2015'!G9="n/a",0,'tolls 2015'!G9)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W7" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X7" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y7" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z7" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA7" s="5">
         <f>IF('tolls 2015'!G9="n/a",0,'tolls 2015'!G9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB7" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC7" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD7" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE7" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF7" s="5">
         <f>IF('tolls 2015'!V9="n/a",0,'tolls 2015'!V9)*CPI_2015_to_2000</f>
@@ -13548,43 +13611,43 @@
       </c>
       <c r="G9" s="5">
         <f>IF('tolls 2015'!G11="n/a",0,'tolls 2015'!G11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H9" s="5">
         <f>IF('tolls 2015'!H11="n/a",0,'tolls 2015'!H11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I9" s="5">
         <f>IF('tolls 2015'!I11="n/a",0,'tolls 2015'!I11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J9" s="5">
         <f>IF('tolls 2015'!J11="n/a",0,'tolls 2015'!J11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K9" s="5">
         <f>IF('tolls 2015'!K11="n/a",0,'tolls 2015'!K11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L9" s="5">
         <f>IF('tolls 2015'!L11="n/a",0,'tolls 2015'!L11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="M9" s="5">
         <f>IF('tolls 2015'!M11="n/a",0,'tolls 2015'!M11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="N9" s="5">
         <f>IF('tolls 2015'!N11="n/a",0,'tolls 2015'!N11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="O9" s="5">
         <f>IF('tolls 2015'!O11="n/a",0,'tolls 2015'!O11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="P9" s="5">
         <f>IF('tolls 2015'!P11="n/a",0,'tolls 2015'!P11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="Q9" s="5">
         <f>IF('tolls 2015'!Q11="n/a",0,'tolls 2015'!Q11)*CPI_2015_to_2000</f>
@@ -13608,43 +13671,43 @@
       </c>
       <c r="V9" s="5">
         <f>IF('tolls 2015'!G11="n/a",0,'tolls 2015'!G11)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W9" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X9" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y9" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z9" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA9" s="5">
         <f>IF('tolls 2015'!G11="n/a",0,'tolls 2015'!G11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB9" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC9" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD9" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE9" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF9" s="5">
         <f>IF('tolls 2015'!V11="n/a",0,'tolls 2015'!V11)*CPI_2015_to_2000</f>
@@ -13884,43 +13947,43 @@
       </c>
       <c r="G11" s="5">
         <f>IF('tolls 2015'!G13="n/a",0,'tolls 2015'!G13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="H11" s="5">
         <f>IF('tolls 2015'!H13="n/a",0,'tolls 2015'!H13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.1958041958041967</v>
       </c>
       <c r="I11" s="5">
         <f>IF('tolls 2015'!I13="n/a",0,'tolls 2015'!I13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="J11" s="5">
         <f>IF('tolls 2015'!J13="n/a",0,'tolls 2015'!J13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.1958041958041967</v>
       </c>
       <c r="K11" s="5">
         <f>IF('tolls 2015'!K13="n/a",0,'tolls 2015'!K13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="L11" s="5">
         <f>IF('tolls 2015'!L13="n/a",0,'tolls 2015'!L13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="M11" s="5">
         <f>IF('tolls 2015'!M13="n/a",0,'tolls 2015'!M13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.1958041958041967</v>
       </c>
       <c r="N11" s="5">
         <f>IF('tolls 2015'!N13="n/a",0,'tolls 2015'!N13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="O11" s="5">
         <f>IF('tolls 2015'!O13="n/a",0,'tolls 2015'!O13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.1958041958041967</v>
       </c>
       <c r="P11" s="5">
         <f>IF('tolls 2015'!P13="n/a",0,'tolls 2015'!P13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="Q11" s="5">
         <f>IF('tolls 2015'!Q13="n/a",0,'tolls 2015'!Q13)*CPI_2015_to_2000</f>
@@ -13944,43 +14007,43 @@
       </c>
       <c r="V11" s="5">
         <f>IF('tolls 2015'!G13="n/a",0,'tolls 2015'!G13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W11" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X11" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y11" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z11" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA11" s="5">
         <f>IF('tolls 2015'!G13="n/a",0,'tolls 2015'!G13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="AB11" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="AC11" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="AD11" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="AE11" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="AF11" s="5">
         <f>IF('tolls 2015'!V13="n/a",0,'tolls 2015'!V13)*CPI_2015_to_2000</f>
@@ -14220,43 +14283,43 @@
       </c>
       <c r="G13" s="5">
         <f>IF('tolls 2015'!G15="n/a",0,'tolls 2015'!G15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="H13" s="5">
         <f>IF('tolls 2015'!H15="n/a",0,'tolls 2015'!H15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="I13" s="5">
         <f>IF('tolls 2015'!I15="n/a",0,'tolls 2015'!I15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="J13" s="5">
         <f>IF('tolls 2015'!J15="n/a",0,'tolls 2015'!J15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="K13" s="5">
         <f>IF('tolls 2015'!K15="n/a",0,'tolls 2015'!K15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="L13" s="5">
         <f>IF('tolls 2015'!L15="n/a",0,'tolls 2015'!L15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="M13" s="5">
         <f>IF('tolls 2015'!M15="n/a",0,'tolls 2015'!M15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="N13" s="5">
         <f>IF('tolls 2015'!N15="n/a",0,'tolls 2015'!N15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="O13" s="5">
         <f>IF('tolls 2015'!O15="n/a",0,'tolls 2015'!O15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="P13" s="5">
         <f>IF('tolls 2015'!P15="n/a",0,'tolls 2015'!P15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="Q13" s="5">
         <f>IF('tolls 2015'!Q15="n/a",0,'tolls 2015'!Q15)*CPI_2015_to_2000</f>
@@ -14280,43 +14343,43 @@
       </c>
       <c r="V13" s="5">
         <f>IF('tolls 2015'!G15="n/a",0,'tolls 2015'!G15)</f>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="W13" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="X13" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="Y13" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="Z13" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="AA13" s="5">
         <f>IF('tolls 2015'!G15="n/a",0,'tolls 2015'!G15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="AB13" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="AC13" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="AD13" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="AE13" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="AF13" s="5">
         <f>IF('tolls 2015'!V15="n/a",0,'tolls 2015'!V15)*CPI_2015_to_2000</f>
@@ -14556,23 +14619,23 @@
       </c>
       <c r="G15" s="5">
         <f>IF('tolls 2015'!G17="n/a",0,'tolls 2015'!G17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H15" s="5">
         <f>IF('tolls 2015'!H17="n/a",0,'tolls 2015'!H17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I15" s="5">
         <f>IF('tolls 2015'!I17="n/a",0,'tolls 2015'!I17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J15" s="5">
         <f>IF('tolls 2015'!J17="n/a",0,'tolls 2015'!J17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K15" s="5">
         <f>IF('tolls 2015'!K17="n/a",0,'tolls 2015'!K17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L15" s="5">
         <f>IF('tolls 2015'!L17="n/a",0,'tolls 2015'!L17)*CPI_2015_to_2000</f>
@@ -14616,43 +14679,43 @@
       </c>
       <c r="V15" s="5">
         <f>IF('tolls 2015'!G17="n/a",0,'tolls 2015'!G17)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W15" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X15" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y15" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z15" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA15" s="5">
         <f>IF('tolls 2015'!G17="n/a",0,'tolls 2015'!G17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB15" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC15" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD15" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE15" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF15" s="5">
         <f>IF('tolls 2015'!V17="n/a",0,'tolls 2015'!V17)*CPI_2015_to_2000</f>
@@ -14892,23 +14955,23 @@
       </c>
       <c r="G17" s="5">
         <f>IF('tolls 2015'!G19="n/a",0,'tolls 2015'!G19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H17" s="5">
         <f>IF('tolls 2015'!H19="n/a",0,'tolls 2015'!H19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I17" s="5">
         <f>IF('tolls 2015'!I19="n/a",0,'tolls 2015'!I19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J17" s="5">
         <f>IF('tolls 2015'!J19="n/a",0,'tolls 2015'!J19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K17" s="5">
         <f>IF('tolls 2015'!K19="n/a",0,'tolls 2015'!K19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L17" s="5">
         <f>IF('tolls 2015'!L19="n/a",0,'tolls 2015'!L19)*CPI_2015_to_2000</f>
@@ -14952,43 +15015,43 @@
       </c>
       <c r="V17" s="5">
         <f>IF('tolls 2015'!G19="n/a",0,'tolls 2015'!G19)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W17" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X17" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y17" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z17" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA17" s="5">
         <f>IF('tolls 2015'!G19="n/a",0,'tolls 2015'!G19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB17" s="5">
         <f t="shared" ref="AB17" si="17">AA17</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC17" s="5">
         <f t="shared" ref="AC17" si="18">AA17</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD17" s="5">
         <f t="shared" ref="AD17" si="19">AA17</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE17" s="5">
         <f t="shared" ref="AE17" si="20">AA17</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF17" s="5">
         <f>IF('tolls 2015'!V19="n/a",0,'tolls 2015'!V19)</f>
@@ -15872,7 +15935,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
@@ -16236,43 +16299,43 @@
       </c>
       <c r="G3" s="5">
         <f>IF('tolls 2015'!G5="n/a",0,'tolls 2015'!G5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H3" s="5">
         <f>IF('tolls 2015'!H5="n/a",0,'tolls 2015'!H5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I3" s="5">
         <f>IF('tolls 2015'!I5="n/a",0,'tolls 2015'!I5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J3" s="5">
         <f>IF('tolls 2015'!J5="n/a",0,'tolls 2015'!J5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K3" s="5">
         <f>IF('tolls 2015'!K5="n/a",0,'tolls 2015'!K5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L3" s="5">
         <f>IF('tolls 2015'!L5="n/a",0,'tolls 2015'!L5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="M3" s="5">
         <f>IF('tolls 2015'!M5="n/a",0,'tolls 2015'!M5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="N3" s="5">
         <f>IF('tolls 2015'!N5="n/a",0,'tolls 2015'!N5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="O3" s="5">
         <f>IF('tolls 2015'!O5="n/a",0,'tolls 2015'!O5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="P3" s="5">
         <f>IF('tolls 2015'!P5="n/a",0,'tolls 2015'!P5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="Q3" s="5">
         <f>IF('tolls 2015'!Q5="n/a",0,'tolls 2015'!Q5)*CPI_2015_to_2000</f>
@@ -16296,43 +16359,43 @@
       </c>
       <c r="V3" s="5">
         <f>IF('tolls 2015'!G5="n/a",0,'tolls 2015'!G5)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W3" s="5">
         <f t="shared" ref="W3:W17" si="1">V3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X3" s="5">
         <f t="shared" ref="X3:X17" si="2">V3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y3" s="5">
         <f t="shared" ref="Y3:Y17" si="3">V3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="5">
         <f t="shared" ref="Z3:Z17" si="4">V3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA3" s="5">
         <f>IF('tolls 2015'!G5="n/a",0,'tolls 2015'!G5)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB3" s="5">
         <f t="shared" ref="AB3:AB17" si="5">AA3</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC3" s="5">
         <f t="shared" ref="AC3:AC17" si="6">AA3</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD3" s="5">
         <f t="shared" ref="AD3:AD17" si="7">AA3</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE3" s="5">
         <f t="shared" ref="AE3:AE17" si="8">AA3</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF3" s="5">
         <f>IF('tolls 2015'!V5="n/a",0,'tolls 2015'!V5)*CPI_2015_to_2000</f>
@@ -16566,43 +16629,43 @@
       </c>
       <c r="G5" s="5">
         <f>IF('tolls 2015'!G7="n/a",0,'tolls 2015'!G7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H5" s="5">
         <f>IF('tolls 2015'!H7="n/a",0,'tolls 2015'!H7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I5" s="5">
         <f>IF('tolls 2015'!I7="n/a",0,'tolls 2015'!I7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J5" s="5">
         <f>IF('tolls 2015'!J7="n/a",0,'tolls 2015'!J7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K5" s="5">
         <f>IF('tolls 2015'!K7="n/a",0,'tolls 2015'!K7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L5" s="5">
         <f>IF('tolls 2015'!L7="n/a",0,'tolls 2015'!L7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="M5" s="5">
         <f>IF('tolls 2015'!M7="n/a",0,'tolls 2015'!M7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="N5" s="5">
         <f>IF('tolls 2015'!N7="n/a",0,'tolls 2015'!N7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="O5" s="5">
         <f>IF('tolls 2015'!O7="n/a",0,'tolls 2015'!O7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="P5" s="5">
         <f>IF('tolls 2015'!P7="n/a",0,'tolls 2015'!P7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="Q5" s="5">
         <f>IF('tolls 2015'!Q7="n/a",0,'tolls 2015'!Q7)*CPI_2015_to_2000</f>
@@ -16626,43 +16689,43 @@
       </c>
       <c r="V5" s="5">
         <f>IF('tolls 2015'!G7="n/a",0,'tolls 2015'!G7)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W5" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X5" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y5" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z5" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA5" s="5">
         <f>IF('tolls 2015'!G7="n/a",0,'tolls 2015'!G7)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB5" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC5" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD5" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE5" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF5" s="5">
         <f>IF('tolls 2015'!V7="n/a",0,'tolls 2015'!V7)*CPI_2015_to_2000</f>
@@ -16896,43 +16959,43 @@
       </c>
       <c r="G7" s="5">
         <f>IF('tolls 2015'!G9="n/a",0,'tolls 2015'!G9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H7" s="5">
         <f>IF('tolls 2015'!H9="n/a",0,'tolls 2015'!H9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I7" s="5">
         <f>IF('tolls 2015'!I9="n/a",0,'tolls 2015'!I9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J7" s="5">
         <f>IF('tolls 2015'!J9="n/a",0,'tolls 2015'!J9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K7" s="5">
         <f>IF('tolls 2015'!K9="n/a",0,'tolls 2015'!K9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L7" s="5">
         <f>IF('tolls 2015'!L9="n/a",0,'tolls 2015'!L9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="M7" s="5">
         <f>IF('tolls 2015'!M9="n/a",0,'tolls 2015'!M9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="N7" s="5">
         <f>IF('tolls 2015'!N9="n/a",0,'tolls 2015'!N9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="O7" s="5">
         <f>IF('tolls 2015'!O9="n/a",0,'tolls 2015'!O9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="P7" s="5">
         <f>IF('tolls 2015'!P9="n/a",0,'tolls 2015'!P9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="Q7" s="5">
         <f>IF('tolls 2015'!Q9="n/a",0,'tolls 2015'!Q9)*CPI_2015_to_2000</f>
@@ -16956,43 +17019,43 @@
       </c>
       <c r="V7" s="5">
         <f>IF('tolls 2015'!G9="n/a",0,'tolls 2015'!G9)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W7" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X7" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y7" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z7" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA7" s="5">
         <f>IF('tolls 2015'!G9="n/a",0,'tolls 2015'!G9)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB7" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC7" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD7" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE7" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF7" s="5">
         <f>IF('tolls 2015'!V9="n/a",0,'tolls 2015'!V9)*CPI_2015_to_2000</f>
@@ -17226,43 +17289,43 @@
       </c>
       <c r="G9" s="5">
         <f>IF('tolls 2015'!G11="n/a",0,'tolls 2015'!G11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H9" s="5">
         <f>IF('tolls 2015'!H11="n/a",0,'tolls 2015'!H11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I9" s="5">
         <f>IF('tolls 2015'!I11="n/a",0,'tolls 2015'!I11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J9" s="5">
         <f>IF('tolls 2015'!J11="n/a",0,'tolls 2015'!J11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K9" s="5">
         <f>IF('tolls 2015'!K11="n/a",0,'tolls 2015'!K11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L9" s="5">
         <f>IF('tolls 2015'!L11="n/a",0,'tolls 2015'!L11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="M9" s="5">
         <f>IF('tolls 2015'!M11="n/a",0,'tolls 2015'!M11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="N9" s="5">
         <f>IF('tolls 2015'!N11="n/a",0,'tolls 2015'!N11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="O9" s="5">
         <f>IF('tolls 2015'!O11="n/a",0,'tolls 2015'!O11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="P9" s="5">
         <f>IF('tolls 2015'!P11="n/a",0,'tolls 2015'!P11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="Q9" s="5">
         <f>IF('tolls 2015'!Q11="n/a",0,'tolls 2015'!Q11)*CPI_2015_to_2000</f>
@@ -17286,43 +17349,43 @@
       </c>
       <c r="V9" s="5">
         <f>IF('tolls 2015'!G11="n/a",0,'tolls 2015'!G11)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W9" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X9" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y9" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z9" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA9" s="5">
         <f>IF('tolls 2015'!G11="n/a",0,'tolls 2015'!G11)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB9" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC9" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD9" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE9" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF9" s="5">
         <f>IF('tolls 2015'!V11="n/a",0,'tolls 2015'!V11)*CPI_2015_to_2000</f>
@@ -17556,43 +17619,43 @@
       </c>
       <c r="G11" s="5">
         <f>IF('tolls 2015'!G13="n/a",0,'tolls 2015'!G13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="H11" s="5">
         <f>IF('tolls 2015'!H13="n/a",0,'tolls 2015'!H13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.1958041958041967</v>
       </c>
       <c r="I11" s="5">
         <f>IF('tolls 2015'!I13="n/a",0,'tolls 2015'!I13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="J11" s="5">
         <f>IF('tolls 2015'!J13="n/a",0,'tolls 2015'!J13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.1958041958041967</v>
       </c>
       <c r="K11" s="5">
         <f>IF('tolls 2015'!K13="n/a",0,'tolls 2015'!K13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="L11" s="5">
         <f>IF('tolls 2015'!L13="n/a",0,'tolls 2015'!L13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="M11" s="5">
         <f>IF('tolls 2015'!M13="n/a",0,'tolls 2015'!M13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.1958041958041967</v>
       </c>
       <c r="N11" s="5">
         <f>IF('tolls 2015'!N13="n/a",0,'tolls 2015'!N13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="O11" s="5">
         <f>IF('tolls 2015'!O13="n/a",0,'tolls 2015'!O13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.1958041958041967</v>
       </c>
       <c r="P11" s="5">
         <f>IF('tolls 2015'!P13="n/a",0,'tolls 2015'!P13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="Q11" s="5">
         <f>IF('tolls 2015'!Q13="n/a",0,'tolls 2015'!Q13)*CPI_2015_to_2000</f>
@@ -17616,43 +17679,43 @@
       </c>
       <c r="V11" s="5">
         <f>IF('tolls 2015'!G13="n/a",0,'tolls 2015'!G13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W11" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X11" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y11" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z11" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA11" s="5">
         <f>IF('tolls 2015'!G13="n/a",0,'tolls 2015'!G13)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="AB11" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="AC11" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="AD11" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="AE11" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2.7972027972027975</v>
       </c>
       <c r="AF11" s="5">
         <f>IF('tolls 2015'!V13="n/a",0,'tolls 2015'!V13)*CPI_2015_to_2000</f>
@@ -17886,43 +17949,43 @@
       </c>
       <c r="G13" s="5">
         <f>IF('tolls 2015'!G15="n/a",0,'tolls 2015'!G15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="H13" s="5">
         <f>IF('tolls 2015'!H15="n/a",0,'tolls 2015'!H15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="I13" s="5">
         <f>IF('tolls 2015'!I15="n/a",0,'tolls 2015'!I15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="J13" s="5">
         <f>IF('tolls 2015'!J15="n/a",0,'tolls 2015'!J15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="K13" s="5">
         <f>IF('tolls 2015'!K15="n/a",0,'tolls 2015'!K15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="L13" s="5">
         <f>IF('tolls 2015'!L15="n/a",0,'tolls 2015'!L15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="M13" s="5">
         <f>IF('tolls 2015'!M15="n/a",0,'tolls 2015'!M15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="N13" s="5">
         <f>IF('tolls 2015'!N15="n/a",0,'tolls 2015'!N15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="O13" s="5">
         <f>IF('tolls 2015'!O15="n/a",0,'tolls 2015'!O15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="P13" s="5">
         <f>IF('tolls 2015'!P15="n/a",0,'tolls 2015'!P15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="Q13" s="5">
         <f>IF('tolls 2015'!Q15="n/a",0,'tolls 2015'!Q15)*CPI_2015_to_2000</f>
@@ -17946,43 +18009,43 @@
       </c>
       <c r="V13" s="5">
         <f>IF('tolls 2015'!G15="n/a",0,'tolls 2015'!G15)</f>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="W13" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="X13" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="Y13" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="Z13" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="AA13" s="5">
         <f>IF('tolls 2015'!G15="n/a",0,'tolls 2015'!G15)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="AB13" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="AC13" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="AD13" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="AE13" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>4.7202797202797209</v>
       </c>
       <c r="AF13" s="5">
         <f>IF('tolls 2015'!V15="n/a",0,'tolls 2015'!V15)*CPI_2015_to_2000</f>
@@ -18216,23 +18279,23 @@
       </c>
       <c r="G15" s="5">
         <f>IF('tolls 2015'!G17="n/a",0,'tolls 2015'!G17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H15" s="5">
         <f>IF('tolls 2015'!H17="n/a",0,'tolls 2015'!H17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I15" s="5">
         <f>IF('tolls 2015'!I17="n/a",0,'tolls 2015'!I17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J15" s="5">
         <f>IF('tolls 2015'!J17="n/a",0,'tolls 2015'!J17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K15" s="5">
         <f>IF('tolls 2015'!K17="n/a",0,'tolls 2015'!K17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L15" s="5">
         <f>IF('tolls 2015'!L17="n/a",0,'tolls 2015'!L17)*CPI_2015_to_2000</f>
@@ -18276,43 +18339,43 @@
       </c>
       <c r="V15" s="5">
         <f>IF('tolls 2015'!G17="n/a",0,'tolls 2015'!G17)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W15" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X15" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y15" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z15" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA15" s="5">
         <f>IF('tolls 2015'!G17="n/a",0,'tolls 2015'!G17)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB15" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC15" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD15" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE15" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF15" s="5">
         <f>IF('tolls 2015'!V17="n/a",0,'tolls 2015'!V17)*CPI_2015_to_2000</f>
@@ -18546,23 +18609,23 @@
       </c>
       <c r="G17" s="5">
         <f>IF('tolls 2015'!G19="n/a",0,'tolls 2015'!G19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="H17" s="5">
         <f>IF('tolls 2015'!H19="n/a",0,'tolls 2015'!H19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="I17" s="5">
         <f>IF('tolls 2015'!I19="n/a",0,'tolls 2015'!I19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="J17" s="5">
         <f>IF('tolls 2015'!J19="n/a",0,'tolls 2015'!J19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="K17" s="5">
         <f>IF('tolls 2015'!K19="n/a",0,'tolls 2015'!K19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="L17" s="5">
         <f>IF('tolls 2015'!L19="n/a",0,'tolls 2015'!L19)*CPI_2015_to_2000</f>
@@ -18606,43 +18669,43 @@
       </c>
       <c r="V17" s="5">
         <f>IF('tolls 2015'!G19="n/a",0,'tolls 2015'!G19)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W17" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X17" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y17" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z17" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA17" s="5">
         <f>IF('tolls 2015'!G19="n/a",0,'tolls 2015'!G19)*CPI_2015_to_2000</f>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AB17" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AC17" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AD17" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AE17" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3.4965034965034967</v>
       </c>
       <c r="AF17" s="5">
         <f>IF('tolls 2015'!V19="n/a",0,'tolls 2015'!V19)</f>
@@ -21581,7 +21644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21607,7 +21670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21644,7 +21707,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>